<commit_message>
datos a plantillas excel
</commit_message>
<xml_diff>
--- a/ExcelAddIn1/Resources/FICHA RECETA.xlsx
+++ b/ExcelAddIn1/Resources/FICHA RECETA.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MANOLO\Documents\GitHub\VSTOexcelRest\ExcelAddIn1\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MANOLO\Desktop\JOB\proyecto cocina\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19560" windowHeight="8340" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19560" windowHeight="8340" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ReporteInventario" sheetId="3" r:id="rId1"/>
     <sheet name="ReporteInventarioImprimir" sheetId="4" r:id="rId2"/>
     <sheet name="Receta" sheetId="1" r:id="rId3"/>
     <sheet name="ReporterCocina" sheetId="5" r:id="rId4"/>
+    <sheet name="DetalleReceta" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="CANTIDAD_A_ELABORAR">Receta!$J$4</definedName>
@@ -32,6 +33,8 @@
     <definedName name="NOMBRE">Receta!$B$2</definedName>
     <definedName name="PESO_LITRO">Receta!$J$2</definedName>
     <definedName name="PRECIO_VENTA">Receta!$J$8</definedName>
+    <definedName name="Rece">DetalleReceta!$B$5</definedName>
+    <definedName name="RECETA_KG">DetalleReceta!$B$5</definedName>
     <definedName name="TITULOCANTIDAD">Receta!$A$1</definedName>
     <definedName name="TOLERANCIA_ERROR">Receta!$J$6</definedName>
     <definedName name="UNIDAD_RECETA">Receta!$A$3</definedName>
@@ -44,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="98">
   <si>
     <t>Receta</t>
   </si>
@@ -283,19 +286,96 @@
   </si>
   <si>
     <t>Fecha :</t>
+  </si>
+  <si>
+    <t>Since</t>
+  </si>
+  <si>
+    <t>Tipo Producto</t>
+  </si>
+  <si>
+    <t>Cantidad en Inventario</t>
+  </si>
+  <si>
+    <t>Arroz Primavera</t>
+  </si>
+  <si>
+    <t>Tipo de Producto</t>
+  </si>
+  <si>
+    <t># Menu´s</t>
+  </si>
+  <si>
+    <t>Since QTY</t>
+  </si>
+  <si>
+    <t>Cantidad Elaborada Promedio X Menu</t>
+  </si>
+  <si>
+    <t>Sobrantes Promedio X Menu</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Costo </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Expresado en Medida de Venta)</t>
+    </r>
+  </si>
+  <si>
+    <t>RECETA PARA:</t>
+  </si>
+  <si>
+    <t>Kgs</t>
+  </si>
+  <si>
+    <t>LTS</t>
+  </si>
+  <si>
+    <t>Ultima Elaboracion</t>
+  </si>
+  <si>
+    <t>Densidad</t>
+  </si>
+  <si>
+    <t>Medida para Venta</t>
+  </si>
+  <si>
+    <t>Ingredientes</t>
+  </si>
+  <si>
+    <t>Cantidad</t>
+  </si>
+  <si>
+    <t>FOTO</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Costo Total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="7" formatCode="&quot;$&quot;#,##0.00;\-&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-[$$-80A]* #,##0.00_-;\-[$$-80A]* #,##0.00_-;_-[$$-80A]* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="0.000%"/>
+    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -425,8 +505,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="28"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -493,6 +602,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="38">
     <border>
@@ -957,7 +1072,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="199">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1261,6 +1376,47 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="7" fontId="0" fillId="10" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -1361,52 +1517,231 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="7" fontId="0" fillId="10" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="13" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="13" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="19" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="7" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="8" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1955,45 +2290,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="80" t="s">
+      <c r="B1" s="97" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
       <c r="G1" s="66" t="s">
         <v>54</v>
       </c>
       <c r="H1" s="66"/>
-      <c r="I1" s="81">
+      <c r="I1" s="98">
         <v>42491</v>
       </c>
-      <c r="J1" s="81"/>
+      <c r="J1" s="98"/>
     </row>
     <row r="2" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="80"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
       <c r="G2" s="68" t="s">
         <v>55</v>
       </c>
       <c r="H2" s="68"/>
-      <c r="I2" s="81">
+      <c r="I2" s="98">
         <v>42639</v>
       </c>
-      <c r="J2" s="81"/>
+      <c r="J2" s="98"/>
     </row>
     <row r="3" spans="1:10" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="79" t="s">
+      <c r="B3" s="96" t="s">
         <v>56</v>
       </c>
-      <c r="C3" s="79"/>
-      <c r="D3" s="79"/>
-      <c r="E3" s="79"/>
-      <c r="F3" s="79"/>
+      <c r="C3" s="96"/>
+      <c r="D3" s="96"/>
+      <c r="E3" s="96"/>
+      <c r="F3" s="96"/>
       <c r="G3" s="67"/>
       <c r="H3" s="67"/>
       <c r="I3" s="65"/>
@@ -2133,7 +2468,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -2151,52 +2486,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="92" t="s">
+      <c r="A1" s="109" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="82" t="s">
+      <c r="B1" s="99" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="83"/>
-      <c r="F1" s="84"/>
+      <c r="C1" s="100"/>
+      <c r="D1" s="100"/>
+      <c r="E1" s="100"/>
+      <c r="F1" s="101"/>
       <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="93"/>
-      <c r="B2" s="85" t="s">
+      <c r="A2" s="110"/>
+      <c r="B2" s="102" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="87"/>
-      <c r="G2" s="98" t="s">
+      <c r="C2" s="103"/>
+      <c r="D2" s="103"/>
+      <c r="E2" s="103"/>
+      <c r="F2" s="104"/>
+      <c r="G2" s="115" t="s">
         <v>47</v>
       </c>
-      <c r="H2" s="100" t="s">
+      <c r="H2" s="117" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="101"/>
+      <c r="I2" s="118"/>
       <c r="J2" s="19">
         <v>0.85</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="94"/>
-      <c r="B3" s="88"/>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="99"/>
-      <c r="H3" s="100" t="s">
+      <c r="A3" s="111"/>
+      <c r="B3" s="105"/>
+      <c r="C3" s="106"/>
+      <c r="D3" s="106"/>
+      <c r="E3" s="106"/>
+      <c r="F3" s="107"/>
+      <c r="G3" s="116"/>
+      <c r="H3" s="117" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="101"/>
+      <c r="I3" s="118"/>
       <c r="J3" s="20">
         <v>10</v>
       </c>
@@ -2223,10 +2558,10 @@
       <c r="G4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="102" t="s">
+      <c r="H4" s="119" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="103"/>
+      <c r="I4" s="120"/>
       <c r="J4" s="23">
         <v>8.5</v>
       </c>
@@ -2239,10 +2574,10 @@
       <c r="E5" s="24"/>
       <c r="F5" s="26"/>
       <c r="G5" s="26"/>
-      <c r="H5" s="91" t="s">
+      <c r="H5" s="108" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="95"/>
+      <c r="I5" s="112"/>
       <c r="J5" s="27">
         <f>SUM(G5:G100)</f>
         <v>0</v>
@@ -2256,10 +2591,10 @@
       <c r="E6" s="24"/>
       <c r="F6" s="26"/>
       <c r="G6" s="26"/>
-      <c r="H6" s="91" t="s">
+      <c r="H6" s="108" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="95"/>
+      <c r="I6" s="112"/>
       <c r="J6" s="28">
         <f>J5*0.05</f>
         <v>0</v>
@@ -2273,10 +2608,10 @@
       <c r="E7" s="24"/>
       <c r="F7" s="26"/>
       <c r="G7" s="26"/>
-      <c r="H7" s="91" t="s">
+      <c r="H7" s="108" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="95"/>
+      <c r="I7" s="112"/>
       <c r="J7" s="28">
         <v>110</v>
       </c>
@@ -2289,10 +2624,10 @@
       <c r="E8" s="24"/>
       <c r="F8" s="26"/>
       <c r="G8" s="26"/>
-      <c r="H8" s="91" t="s">
+      <c r="H8" s="108" t="s">
         <v>14</v>
       </c>
-      <c r="I8" s="95"/>
+      <c r="I8" s="112"/>
       <c r="J8" s="29">
         <v>150</v>
       </c>
@@ -2305,10 +2640,10 @@
       <c r="E9" s="24"/>
       <c r="F9" s="26"/>
       <c r="G9" s="26"/>
-      <c r="H9" s="91" t="s">
+      <c r="H9" s="108" t="s">
         <v>15</v>
       </c>
-      <c r="I9" s="91"/>
+      <c r="I9" s="108"/>
       <c r="J9" s="30">
         <f>(PRECIO_VENTA*LITROS_A_ELABORAR)</f>
         <v>1500</v>
@@ -2322,10 +2657,10 @@
       <c r="E10" s="24"/>
       <c r="F10" s="26"/>
       <c r="G10" s="26"/>
-      <c r="H10" s="91" t="s">
+      <c r="H10" s="108" t="s">
         <v>16</v>
       </c>
-      <c r="I10" s="91"/>
+      <c r="I10" s="108"/>
       <c r="J10" s="31">
         <f>J9-COSTO_TOTAL_MATERIA_PRIMA</f>
         <v>1500</v>
@@ -2339,10 +2674,10 @@
       <c r="E11" s="24"/>
       <c r="F11" s="26"/>
       <c r="G11" s="26"/>
-      <c r="H11" s="96" t="s">
+      <c r="H11" s="113" t="s">
         <v>19</v>
       </c>
-      <c r="I11" s="97"/>
+      <c r="I11" s="114"/>
       <c r="J11" s="32">
         <v>0.27</v>
       </c>
@@ -2355,10 +2690,10 @@
       <c r="E12" s="24"/>
       <c r="F12" s="26"/>
       <c r="G12" s="26"/>
-      <c r="H12" s="96" t="s">
+      <c r="H12" s="113" t="s">
         <v>20</v>
       </c>
-      <c r="I12" s="97"/>
+      <c r="I12" s="114"/>
       <c r="J12" s="32">
         <f>((J5+COSTO_PREPARACION)/J9-1)*(-1)</f>
         <v>0.92666666666666664</v>
@@ -2461,669 +2796,1165 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z25"/>
+  <dimension ref="A1:AC25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="X12" sqref="X12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" customWidth="1"/>
-    <col min="12" max="12" width="23.5703125" customWidth="1"/>
-    <col min="13" max="13" width="15.85546875" customWidth="1"/>
+    <col min="2" max="4" width="17.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" customWidth="1"/>
+    <col min="15" max="15" width="23.5703125" customWidth="1"/>
+    <col min="16" max="16" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="122" t="s">
+    <row r="1" spans="1:29" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="95" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="121">
+      <c r="B1" s="94">
         <v>42811</v>
       </c>
-      <c r="C1" s="106"/>
-      <c r="D1" s="106"/>
-      <c r="E1" s="106"/>
-      <c r="F1" s="106"/>
-      <c r="G1" s="106"/>
-      <c r="H1" s="106"/>
-      <c r="I1" s="106"/>
-      <c r="J1" s="106"/>
-      <c r="K1" s="106"/>
-      <c r="L1" s="106"/>
-      <c r="M1" s="106"/>
-      <c r="N1" s="119" t="s">
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
+      <c r="H1" s="81"/>
+      <c r="I1" s="81"/>
+      <c r="J1" s="81"/>
+      <c r="K1" s="81"/>
+      <c r="L1" s="81"/>
+      <c r="M1" s="81"/>
+      <c r="N1" s="81"/>
+      <c r="O1" s="81"/>
+      <c r="P1" s="81"/>
+      <c r="Q1" s="121" t="s">
         <v>60</v>
       </c>
-      <c r="O1" s="120"/>
-      <c r="P1" s="119" t="s">
+      <c r="R1" s="122"/>
+      <c r="S1" s="121" t="s">
         <v>61</v>
       </c>
-      <c r="Q1" s="120"/>
-      <c r="R1" s="119" t="s">
+      <c r="T1" s="122"/>
+      <c r="U1" s="121" t="s">
         <v>62</v>
       </c>
-      <c r="S1" s="120"/>
-      <c r="T1" s="119" t="s">
+      <c r="V1" s="122"/>
+      <c r="W1" s="121" t="s">
         <v>63</v>
       </c>
-      <c r="U1" s="120"/>
-      <c r="V1" s="106"/>
-      <c r="W1" s="106"/>
-      <c r="X1" s="106"/>
-      <c r="Y1" s="106"/>
-      <c r="Z1" s="106"/>
-    </row>
-    <row r="2" spans="1:26" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="115" t="s">
+      <c r="X1" s="122"/>
+      <c r="Y1" s="81"/>
+      <c r="Z1" s="81"/>
+      <c r="AA1" s="81"/>
+      <c r="AB1" s="81"/>
+      <c r="AC1" s="81"/>
+    </row>
+    <row r="2" spans="1:29" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="90" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="116" t="s">
+      <c r="B2" s="91" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="116" t="s">
+      <c r="C2" s="91" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" s="91" t="s">
+        <v>79</v>
+      </c>
+      <c r="E2" s="91" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="116" t="s">
+      <c r="F2" s="91" t="s">
         <v>59</v>
       </c>
-      <c r="E2" s="116" t="s">
+      <c r="G2" s="91" t="s">
+        <v>77</v>
+      </c>
+      <c r="H2" s="91" t="s">
         <v>75</v>
       </c>
-      <c r="F2" s="116" t="s">
+      <c r="I2" s="91" t="s">
         <v>67</v>
       </c>
-      <c r="G2" s="116" t="s">
+      <c r="J2" s="91" t="s">
         <v>74</v>
       </c>
-      <c r="H2" s="116" t="s">
+      <c r="K2" s="91" t="s">
         <v>69</v>
       </c>
-      <c r="I2" s="116" t="s">
+      <c r="L2" s="91" t="s">
         <v>70</v>
       </c>
-      <c r="J2" s="116" t="s">
+      <c r="M2" s="91" t="s">
         <v>35</v>
       </c>
-      <c r="K2" s="116" t="s">
+      <c r="N2" s="91" t="s">
         <v>68</v>
       </c>
-      <c r="L2" s="116" t="s">
+      <c r="O2" s="91" t="s">
         <v>71</v>
       </c>
-      <c r="M2" s="116" t="s">
+      <c r="P2" s="91" t="s">
         <v>72</v>
       </c>
-      <c r="N2" s="108" t="s">
+      <c r="Q2" s="83" t="s">
         <v>64</v>
       </c>
-      <c r="O2" s="109" t="s">
+      <c r="R2" s="84" t="s">
         <v>65</v>
       </c>
-      <c r="P2" s="108" t="s">
+      <c r="S2" s="83" t="s">
         <v>64</v>
       </c>
-      <c r="Q2" s="108" t="s">
+      <c r="T2" s="83" t="s">
         <v>66</v>
       </c>
-      <c r="R2" s="109" t="s">
+      <c r="U2" s="84" t="s">
         <v>64</v>
       </c>
-      <c r="S2" s="108" t="s">
+      <c r="V2" s="83" t="s">
         <v>66</v>
       </c>
-      <c r="T2" s="108" t="s">
+      <c r="W2" s="83" t="s">
         <v>64</v>
       </c>
-      <c r="U2" s="108" t="s">
+      <c r="X2" s="83" t="s">
         <v>66</v>
       </c>
-      <c r="V2" s="107"/>
-      <c r="W2" s="107"/>
-      <c r="X2" s="107"/>
-      <c r="Y2" s="107"/>
-      <c r="Z2" s="107"/>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A3" s="110"/>
-      <c r="B3" s="110"/>
-      <c r="C3" s="110"/>
-      <c r="D3" s="110"/>
-      <c r="E3" s="110"/>
-      <c r="F3" s="110"/>
-      <c r="G3" s="110"/>
-      <c r="H3" s="117"/>
-      <c r="I3" s="118"/>
-      <c r="J3" s="110"/>
-      <c r="K3" s="110"/>
-      <c r="L3" s="111"/>
-      <c r="M3" s="111"/>
-      <c r="N3" s="105"/>
-      <c r="O3" s="113"/>
-      <c r="P3" s="105"/>
-      <c r="Q3" s="114"/>
-      <c r="R3" s="105"/>
-      <c r="S3" s="104"/>
-      <c r="T3" s="105"/>
-      <c r="U3" s="104"/>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A4" s="110"/>
-      <c r="B4" s="110"/>
-      <c r="C4" s="110"/>
-      <c r="D4" s="110"/>
-      <c r="E4" s="110"/>
-      <c r="F4" s="110"/>
-      <c r="G4" s="110"/>
-      <c r="H4" s="117"/>
-      <c r="I4" s="118"/>
-      <c r="J4" s="110"/>
-      <c r="K4" s="110"/>
-      <c r="L4" s="111"/>
-      <c r="M4" s="111"/>
-      <c r="N4" s="105"/>
-      <c r="O4" s="113"/>
-      <c r="P4" s="105"/>
-      <c r="Q4" s="114"/>
-      <c r="R4" s="105"/>
-      <c r="S4" s="104"/>
-      <c r="T4" s="105"/>
-      <c r="U4" s="104"/>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A5" s="110"/>
-      <c r="B5" s="110"/>
-      <c r="C5" s="110"/>
-      <c r="D5" s="110"/>
-      <c r="E5" s="110"/>
-      <c r="F5" s="110"/>
-      <c r="G5" s="110"/>
-      <c r="H5" s="117"/>
-      <c r="I5" s="118"/>
-      <c r="J5" s="110"/>
-      <c r="K5" s="110"/>
-      <c r="L5" s="111"/>
-      <c r="M5" s="111"/>
-      <c r="N5" s="105"/>
-      <c r="O5" s="113"/>
-      <c r="P5" s="105"/>
-      <c r="Q5" s="114"/>
-      <c r="R5" s="105"/>
-      <c r="S5" s="104"/>
-      <c r="T5" s="105"/>
-      <c r="U5" s="104"/>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A6" s="110"/>
-      <c r="B6" s="110"/>
-      <c r="C6" s="110"/>
-      <c r="D6" s="110"/>
-      <c r="E6" s="110"/>
-      <c r="F6" s="110"/>
-      <c r="G6" s="110"/>
-      <c r="H6" s="117"/>
-      <c r="I6" s="118"/>
-      <c r="J6" s="110"/>
-      <c r="K6" s="110"/>
-      <c r="L6" s="112"/>
-      <c r="M6" s="112"/>
-      <c r="N6" s="110"/>
-      <c r="O6" s="110"/>
-      <c r="P6" s="110"/>
-      <c r="Q6" s="110"/>
-      <c r="R6" s="110"/>
-      <c r="S6" s="110"/>
-      <c r="T6" s="110"/>
-      <c r="U6" s="110"/>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A7" s="110"/>
-      <c r="B7" s="110"/>
-      <c r="C7" s="110"/>
-      <c r="D7" s="110"/>
-      <c r="E7" s="110"/>
-      <c r="F7" s="110"/>
-      <c r="G7" s="110"/>
-      <c r="H7" s="117"/>
-      <c r="I7" s="118"/>
-      <c r="J7" s="110"/>
-      <c r="K7" s="110"/>
-      <c r="L7" s="112"/>
-      <c r="M7" s="112"/>
-      <c r="N7" s="110"/>
-      <c r="O7" s="110"/>
-      <c r="P7" s="110"/>
-      <c r="Q7" s="110"/>
-      <c r="R7" s="110"/>
-      <c r="S7" s="110"/>
-      <c r="T7" s="110"/>
-      <c r="U7" s="110"/>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A8" s="110"/>
-      <c r="B8" s="110"/>
-      <c r="C8" s="110"/>
-      <c r="D8" s="110"/>
-      <c r="E8" s="110"/>
-      <c r="F8" s="110"/>
-      <c r="G8" s="110"/>
-      <c r="H8" s="117"/>
-      <c r="I8" s="118"/>
-      <c r="J8" s="110"/>
-      <c r="K8" s="110"/>
-      <c r="L8" s="112"/>
-      <c r="M8" s="112"/>
-      <c r="N8" s="110"/>
-      <c r="O8" s="110"/>
-      <c r="P8" s="110"/>
-      <c r="Q8" s="110"/>
-      <c r="R8" s="110"/>
-      <c r="S8" s="110"/>
-      <c r="T8" s="110"/>
-      <c r="U8" s="110"/>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A9" s="110"/>
-      <c r="B9" s="110"/>
-      <c r="C9" s="110"/>
-      <c r="D9" s="110"/>
-      <c r="E9" s="110"/>
-      <c r="F9" s="110"/>
-      <c r="G9" s="110"/>
-      <c r="H9" s="117"/>
-      <c r="I9" s="118"/>
-      <c r="J9" s="110"/>
-      <c r="K9" s="110"/>
-      <c r="L9" s="112"/>
-      <c r="M9" s="112"/>
-      <c r="N9" s="110"/>
-      <c r="O9" s="110"/>
-      <c r="P9" s="110"/>
-      <c r="Q9" s="110"/>
-      <c r="R9" s="110"/>
-      <c r="S9" s="110"/>
-      <c r="T9" s="110"/>
-      <c r="U9" s="110"/>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A10" s="110"/>
-      <c r="B10" s="110"/>
-      <c r="C10" s="110"/>
-      <c r="D10" s="110"/>
-      <c r="E10" s="110"/>
-      <c r="F10" s="110"/>
-      <c r="G10" s="110"/>
-      <c r="H10" s="117"/>
-      <c r="I10" s="118"/>
-      <c r="J10" s="110"/>
-      <c r="K10" s="110"/>
-      <c r="L10" s="112"/>
-      <c r="M10" s="112"/>
-      <c r="N10" s="110"/>
-      <c r="O10" s="110"/>
-      <c r="P10" s="110"/>
-      <c r="Q10" s="110"/>
-      <c r="R10" s="110"/>
-      <c r="S10" s="110"/>
-      <c r="T10" s="110"/>
-      <c r="U10" s="110"/>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A11" s="110"/>
-      <c r="B11" s="110"/>
-      <c r="C11" s="110"/>
-      <c r="D11" s="110"/>
-      <c r="E11" s="110"/>
-      <c r="F11" s="110"/>
-      <c r="G11" s="110"/>
-      <c r="H11" s="117"/>
-      <c r="I11" s="118"/>
-      <c r="J11" s="110"/>
-      <c r="K11" s="110"/>
-      <c r="L11" s="112"/>
-      <c r="M11" s="112"/>
-      <c r="N11" s="110"/>
-      <c r="O11" s="110"/>
-      <c r="P11" s="110"/>
-      <c r="Q11" s="110"/>
-      <c r="R11" s="110"/>
-      <c r="S11" s="110"/>
-      <c r="T11" s="110"/>
-      <c r="U11" s="110"/>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A12" s="110"/>
-      <c r="B12" s="110"/>
-      <c r="C12" s="110"/>
-      <c r="D12" s="110"/>
-      <c r="E12" s="110"/>
-      <c r="F12" s="110"/>
-      <c r="G12" s="110"/>
-      <c r="H12" s="117"/>
-      <c r="I12" s="118"/>
-      <c r="J12" s="110"/>
-      <c r="K12" s="110"/>
-      <c r="L12" s="112"/>
-      <c r="M12" s="112"/>
-      <c r="N12" s="110"/>
-      <c r="O12" s="110"/>
-      <c r="P12" s="110"/>
-      <c r="Q12" s="110"/>
-      <c r="R12" s="110"/>
-      <c r="S12" s="110"/>
-      <c r="T12" s="110"/>
-      <c r="U12" s="110"/>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A13" s="110"/>
-      <c r="B13" s="110"/>
-      <c r="C13" s="110"/>
-      <c r="D13" s="110"/>
-      <c r="E13" s="110"/>
-      <c r="F13" s="110"/>
-      <c r="G13" s="110"/>
-      <c r="H13" s="117"/>
-      <c r="I13" s="118"/>
-      <c r="J13" s="110"/>
-      <c r="K13" s="110"/>
-      <c r="L13" s="112"/>
-      <c r="M13" s="112"/>
-      <c r="N13" s="110"/>
-      <c r="O13" s="110"/>
-      <c r="P13" s="110"/>
-      <c r="Q13" s="110"/>
-      <c r="R13" s="110"/>
-      <c r="S13" s="110"/>
-      <c r="T13" s="110"/>
-      <c r="U13" s="110"/>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A14" s="110"/>
-      <c r="B14" s="110"/>
-      <c r="C14" s="110"/>
-      <c r="D14" s="110"/>
-      <c r="E14" s="110"/>
-      <c r="F14" s="110"/>
-      <c r="G14" s="110"/>
-      <c r="H14" s="117"/>
-      <c r="I14" s="118"/>
-      <c r="J14" s="110"/>
-      <c r="K14" s="110"/>
-      <c r="L14" s="112"/>
-      <c r="M14" s="112"/>
-      <c r="N14" s="110"/>
-      <c r="O14" s="110"/>
-      <c r="P14" s="110"/>
-      <c r="Q14" s="110"/>
-      <c r="R14" s="110"/>
-      <c r="S14" s="110"/>
-      <c r="T14" s="110"/>
-      <c r="U14" s="110"/>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A15" s="110"/>
-      <c r="B15" s="110"/>
-      <c r="C15" s="110"/>
-      <c r="D15" s="110"/>
-      <c r="E15" s="110"/>
-      <c r="F15" s="110"/>
-      <c r="G15" s="110"/>
-      <c r="H15" s="117"/>
-      <c r="I15" s="118"/>
-      <c r="J15" s="110"/>
-      <c r="K15" s="110"/>
-      <c r="L15" s="112"/>
-      <c r="M15" s="112"/>
-      <c r="N15" s="110"/>
-      <c r="O15" s="110"/>
-      <c r="P15" s="110"/>
-      <c r="Q15" s="110"/>
-      <c r="R15" s="110"/>
-      <c r="S15" s="110"/>
-      <c r="T15" s="110"/>
-      <c r="U15" s="110"/>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A16" s="110"/>
-      <c r="B16" s="110"/>
-      <c r="C16" s="110"/>
-      <c r="D16" s="110"/>
-      <c r="E16" s="110"/>
-      <c r="F16" s="110"/>
-      <c r="G16" s="110"/>
-      <c r="H16" s="117"/>
-      <c r="I16" s="118"/>
-      <c r="J16" s="110"/>
-      <c r="K16" s="110"/>
-      <c r="L16" s="112"/>
-      <c r="M16" s="112"/>
-      <c r="N16" s="110"/>
-      <c r="O16" s="110"/>
-      <c r="P16" s="110"/>
-      <c r="Q16" s="110"/>
-      <c r="R16" s="110"/>
-      <c r="S16" s="110"/>
-      <c r="T16" s="110"/>
-      <c r="U16" s="110"/>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A17" s="110"/>
-      <c r="B17" s="110"/>
-      <c r="C17" s="110"/>
-      <c r="D17" s="110"/>
-      <c r="E17" s="110"/>
-      <c r="F17" s="110"/>
-      <c r="G17" s="110"/>
-      <c r="H17" s="117"/>
-      <c r="I17" s="118"/>
-      <c r="J17" s="110"/>
-      <c r="K17" s="110"/>
-      <c r="L17" s="112"/>
-      <c r="M17" s="112"/>
-      <c r="N17" s="110"/>
-      <c r="O17" s="110"/>
-      <c r="P17" s="110"/>
-      <c r="Q17" s="110"/>
-      <c r="R17" s="110"/>
-      <c r="S17" s="110"/>
-      <c r="T17" s="110"/>
-      <c r="U17" s="110"/>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A18" s="110"/>
-      <c r="B18" s="110"/>
-      <c r="C18" s="110"/>
-      <c r="D18" s="110"/>
-      <c r="E18" s="110"/>
-      <c r="F18" s="110"/>
-      <c r="G18" s="110"/>
-      <c r="H18" s="117"/>
-      <c r="I18" s="118"/>
-      <c r="J18" s="110"/>
-      <c r="K18" s="110"/>
-      <c r="L18" s="112"/>
-      <c r="M18" s="112"/>
-      <c r="N18" s="110"/>
-      <c r="O18" s="110"/>
-      <c r="P18" s="110"/>
-      <c r="Q18" s="110"/>
-      <c r="R18" s="110"/>
-      <c r="S18" s="110"/>
-      <c r="T18" s="110"/>
-      <c r="U18" s="110"/>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A19" s="110"/>
-      <c r="B19" s="110"/>
-      <c r="C19" s="110"/>
-      <c r="D19" s="110"/>
-      <c r="E19" s="110"/>
-      <c r="F19" s="110"/>
-      <c r="G19" s="110"/>
-      <c r="H19" s="117"/>
-      <c r="I19" s="118"/>
-      <c r="J19" s="110"/>
-      <c r="K19" s="110"/>
-      <c r="L19" s="112"/>
-      <c r="M19" s="112"/>
-      <c r="N19" s="110"/>
-      <c r="O19" s="110"/>
-      <c r="P19" s="110"/>
-      <c r="Q19" s="110"/>
-      <c r="R19" s="110"/>
-      <c r="S19" s="110"/>
-      <c r="T19" s="110"/>
-      <c r="U19" s="110"/>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A20" s="110"/>
-      <c r="B20" s="110"/>
-      <c r="C20" s="110"/>
-      <c r="D20" s="110"/>
-      <c r="E20" s="110"/>
-      <c r="F20" s="110"/>
-      <c r="G20" s="110"/>
-      <c r="H20" s="117"/>
-      <c r="I20" s="118"/>
-      <c r="J20" s="110"/>
-      <c r="K20" s="110"/>
-      <c r="L20" s="112"/>
-      <c r="M20" s="112"/>
-      <c r="N20" s="110"/>
-      <c r="O20" s="110"/>
-      <c r="P20" s="110"/>
-      <c r="Q20" s="110"/>
-      <c r="R20" s="110"/>
-      <c r="S20" s="110"/>
-      <c r="T20" s="110"/>
-      <c r="U20" s="110"/>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A21" s="110"/>
-      <c r="B21" s="110"/>
-      <c r="C21" s="110"/>
-      <c r="D21" s="110"/>
-      <c r="E21" s="110"/>
-      <c r="F21" s="110"/>
-      <c r="G21" s="110"/>
-      <c r="H21" s="117"/>
-      <c r="I21" s="118"/>
-      <c r="J21" s="110"/>
-      <c r="K21" s="110"/>
-      <c r="L21" s="112"/>
-      <c r="M21" s="112"/>
-      <c r="N21" s="110"/>
-      <c r="O21" s="110"/>
-      <c r="P21" s="110"/>
-      <c r="Q21" s="110"/>
-      <c r="R21" s="110"/>
-      <c r="S21" s="110"/>
-      <c r="T21" s="110"/>
-      <c r="U21" s="110"/>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A22" s="110"/>
-      <c r="B22" s="110"/>
-      <c r="C22" s="110"/>
-      <c r="D22" s="110"/>
-      <c r="E22" s="110"/>
-      <c r="F22" s="110"/>
-      <c r="G22" s="110"/>
-      <c r="H22" s="117"/>
-      <c r="I22" s="118"/>
-      <c r="J22" s="110"/>
-      <c r="K22" s="110"/>
-      <c r="L22" s="112"/>
-      <c r="M22" s="112"/>
-      <c r="N22" s="110"/>
-      <c r="O22" s="110"/>
-      <c r="P22" s="110"/>
-      <c r="Q22" s="110"/>
-      <c r="R22" s="110"/>
-      <c r="S22" s="110"/>
-      <c r="T22" s="110"/>
-      <c r="U22" s="110"/>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A23" s="110"/>
-      <c r="B23" s="110"/>
-      <c r="C23" s="110"/>
-      <c r="D23" s="110"/>
-      <c r="E23" s="110"/>
-      <c r="F23" s="110"/>
-      <c r="G23" s="110"/>
-      <c r="H23" s="117"/>
-      <c r="I23" s="118"/>
-      <c r="J23" s="110"/>
-      <c r="K23" s="110"/>
-      <c r="L23" s="112"/>
-      <c r="M23" s="112"/>
-      <c r="N23" s="110"/>
-      <c r="O23" s="110"/>
-      <c r="P23" s="110"/>
-      <c r="Q23" s="110"/>
-      <c r="R23" s="110"/>
-      <c r="S23" s="110"/>
-      <c r="T23" s="110"/>
-      <c r="U23" s="110"/>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A24" s="110"/>
-      <c r="B24" s="110"/>
-      <c r="C24" s="110"/>
-      <c r="D24" s="110"/>
-      <c r="E24" s="110"/>
-      <c r="F24" s="110"/>
-      <c r="G24" s="110"/>
-      <c r="H24" s="117"/>
-      <c r="I24" s="118"/>
-      <c r="J24" s="110"/>
-      <c r="K24" s="110"/>
-      <c r="L24" s="112"/>
-      <c r="M24" s="112"/>
-      <c r="N24" s="110"/>
-      <c r="O24" s="110"/>
-      <c r="P24" s="110"/>
-      <c r="Q24" s="110"/>
-      <c r="R24" s="110"/>
-      <c r="S24" s="110"/>
-      <c r="T24" s="110"/>
-      <c r="U24" s="110"/>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A25" s="110"/>
-      <c r="B25" s="110"/>
-      <c r="C25" s="110"/>
-      <c r="D25" s="110"/>
-      <c r="E25" s="110"/>
-      <c r="F25" s="110"/>
-      <c r="G25" s="110"/>
-      <c r="H25" s="117"/>
-      <c r="I25" s="118"/>
-      <c r="J25" s="110"/>
-      <c r="K25" s="110"/>
-      <c r="L25" s="112"/>
-      <c r="M25" s="112"/>
-      <c r="N25" s="110"/>
-      <c r="O25" s="110"/>
-      <c r="P25" s="110"/>
-      <c r="Q25" s="110"/>
-      <c r="R25" s="110"/>
-      <c r="S25" s="110"/>
-      <c r="T25" s="110"/>
-      <c r="U25" s="110"/>
+      <c r="Y2" s="82"/>
+      <c r="Z2" s="82"/>
+      <c r="AA2" s="82"/>
+      <c r="AB2" s="82"/>
+      <c r="AC2" s="82"/>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="85"/>
+      <c r="B3" s="85"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="92"/>
+      <c r="L3" s="93"/>
+      <c r="M3" s="85"/>
+      <c r="N3" s="85"/>
+      <c r="O3" s="86"/>
+      <c r="P3" s="86"/>
+      <c r="Q3" s="80"/>
+      <c r="R3" s="88"/>
+      <c r="S3" s="80"/>
+      <c r="T3" s="89"/>
+      <c r="U3" s="80"/>
+      <c r="V3" s="79"/>
+      <c r="W3" s="80"/>
+      <c r="X3" s="79"/>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A4" s="85"/>
+      <c r="B4" s="85"/>
+      <c r="C4" s="85"/>
+      <c r="D4" s="85"/>
+      <c r="E4" s="85"/>
+      <c r="F4" s="85"/>
+      <c r="G4" s="85"/>
+      <c r="H4" s="85"/>
+      <c r="I4" s="85"/>
+      <c r="J4" s="85"/>
+      <c r="K4" s="92"/>
+      <c r="L4" s="93"/>
+      <c r="M4" s="85"/>
+      <c r="N4" s="85"/>
+      <c r="O4" s="86"/>
+      <c r="P4" s="86"/>
+      <c r="Q4" s="80"/>
+      <c r="R4" s="88"/>
+      <c r="S4" s="80"/>
+      <c r="T4" s="89"/>
+      <c r="U4" s="80"/>
+      <c r="V4" s="79"/>
+      <c r="W4" s="80"/>
+      <c r="X4" s="79"/>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A5" s="85"/>
+      <c r="B5" s="85"/>
+      <c r="C5" s="85"/>
+      <c r="D5" s="85"/>
+      <c r="E5" s="85"/>
+      <c r="F5" s="85"/>
+      <c r="G5" s="85"/>
+      <c r="H5" s="85"/>
+      <c r="I5" s="85"/>
+      <c r="J5" s="85"/>
+      <c r="K5" s="92"/>
+      <c r="L5" s="93"/>
+      <c r="M5" s="85"/>
+      <c r="N5" s="85"/>
+      <c r="O5" s="86"/>
+      <c r="P5" s="86"/>
+      <c r="Q5" s="80"/>
+      <c r="R5" s="88"/>
+      <c r="S5" s="80"/>
+      <c r="T5" s="89"/>
+      <c r="U5" s="80"/>
+      <c r="V5" s="79"/>
+      <c r="W5" s="80"/>
+      <c r="X5" s="79"/>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A6" s="85"/>
+      <c r="B6" s="85"/>
+      <c r="C6" s="85"/>
+      <c r="D6" s="85"/>
+      <c r="E6" s="85"/>
+      <c r="F6" s="85"/>
+      <c r="G6" s="85"/>
+      <c r="H6" s="85"/>
+      <c r="I6" s="85"/>
+      <c r="J6" s="85"/>
+      <c r="K6" s="92"/>
+      <c r="L6" s="93"/>
+      <c r="M6" s="85"/>
+      <c r="N6" s="85"/>
+      <c r="O6" s="87"/>
+      <c r="P6" s="87"/>
+      <c r="Q6" s="85"/>
+      <c r="R6" s="85"/>
+      <c r="S6" s="85"/>
+      <c r="T6" s="85"/>
+      <c r="U6" s="85"/>
+      <c r="V6" s="85"/>
+      <c r="W6" s="85"/>
+      <c r="X6" s="85"/>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A7" s="85"/>
+      <c r="B7" s="85"/>
+      <c r="C7" s="85"/>
+      <c r="D7" s="85"/>
+      <c r="E7" s="85"/>
+      <c r="F7" s="85"/>
+      <c r="G7" s="85"/>
+      <c r="H7" s="85"/>
+      <c r="I7" s="85"/>
+      <c r="J7" s="85"/>
+      <c r="K7" s="92"/>
+      <c r="L7" s="93"/>
+      <c r="M7" s="85"/>
+      <c r="N7" s="85"/>
+      <c r="O7" s="87"/>
+      <c r="P7" s="87"/>
+      <c r="Q7" s="85"/>
+      <c r="R7" s="85"/>
+      <c r="S7" s="85"/>
+      <c r="T7" s="85"/>
+      <c r="U7" s="85"/>
+      <c r="V7" s="85"/>
+      <c r="W7" s="85"/>
+      <c r="X7" s="85"/>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A8" s="85"/>
+      <c r="B8" s="85"/>
+      <c r="C8" s="85"/>
+      <c r="D8" s="85"/>
+      <c r="E8" s="85"/>
+      <c r="F8" s="85"/>
+      <c r="G8" s="85"/>
+      <c r="H8" s="85"/>
+      <c r="I8" s="85"/>
+      <c r="J8" s="85"/>
+      <c r="K8" s="92"/>
+      <c r="L8" s="93"/>
+      <c r="M8" s="85"/>
+      <c r="N8" s="85"/>
+      <c r="O8" s="87"/>
+      <c r="P8" s="87"/>
+      <c r="Q8" s="85"/>
+      <c r="R8" s="85"/>
+      <c r="S8" s="85"/>
+      <c r="T8" s="85"/>
+      <c r="U8" s="85"/>
+      <c r="V8" s="85"/>
+      <c r="W8" s="85"/>
+      <c r="X8" s="85"/>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A9" s="85"/>
+      <c r="B9" s="85"/>
+      <c r="C9" s="85"/>
+      <c r="D9" s="85"/>
+      <c r="E9" s="85"/>
+      <c r="F9" s="85"/>
+      <c r="G9" s="85"/>
+      <c r="H9" s="85"/>
+      <c r="I9" s="85"/>
+      <c r="J9" s="85"/>
+      <c r="K9" s="92"/>
+      <c r="L9" s="93"/>
+      <c r="M9" s="85"/>
+      <c r="N9" s="85"/>
+      <c r="O9" s="87"/>
+      <c r="P9" s="87"/>
+      <c r="Q9" s="85"/>
+      <c r="R9" s="85"/>
+      <c r="S9" s="85"/>
+      <c r="T9" s="85"/>
+      <c r="U9" s="85"/>
+      <c r="V9" s="85"/>
+      <c r="W9" s="85"/>
+      <c r="X9" s="85"/>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A10" s="85"/>
+      <c r="B10" s="85"/>
+      <c r="C10" s="85"/>
+      <c r="D10" s="85"/>
+      <c r="E10" s="85"/>
+      <c r="F10" s="85"/>
+      <c r="G10" s="85"/>
+      <c r="H10" s="85"/>
+      <c r="I10" s="85"/>
+      <c r="J10" s="85"/>
+      <c r="K10" s="92"/>
+      <c r="L10" s="93"/>
+      <c r="M10" s="85"/>
+      <c r="N10" s="85"/>
+      <c r="O10" s="87"/>
+      <c r="P10" s="87"/>
+      <c r="Q10" s="85"/>
+      <c r="R10" s="85"/>
+      <c r="S10" s="85"/>
+      <c r="T10" s="85"/>
+      <c r="U10" s="85"/>
+      <c r="V10" s="85"/>
+      <c r="W10" s="85"/>
+      <c r="X10" s="85"/>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A11" s="85"/>
+      <c r="B11" s="85"/>
+      <c r="C11" s="85"/>
+      <c r="D11" s="85"/>
+      <c r="E11" s="85"/>
+      <c r="F11" s="85"/>
+      <c r="G11" s="85"/>
+      <c r="H11" s="85"/>
+      <c r="I11" s="85"/>
+      <c r="J11" s="85"/>
+      <c r="K11" s="92"/>
+      <c r="L11" s="93"/>
+      <c r="M11" s="85"/>
+      <c r="N11" s="85"/>
+      <c r="O11" s="87"/>
+      <c r="P11" s="87"/>
+      <c r="Q11" s="85"/>
+      <c r="R11" s="85"/>
+      <c r="S11" s="85"/>
+      <c r="T11" s="85"/>
+      <c r="U11" s="85"/>
+      <c r="V11" s="85"/>
+      <c r="W11" s="85"/>
+      <c r="X11" s="85"/>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A12" s="85"/>
+      <c r="B12" s="85"/>
+      <c r="C12" s="85"/>
+      <c r="D12" s="85"/>
+      <c r="E12" s="85"/>
+      <c r="F12" s="85"/>
+      <c r="G12" s="85"/>
+      <c r="H12" s="85"/>
+      <c r="I12" s="85"/>
+      <c r="J12" s="85"/>
+      <c r="K12" s="92"/>
+      <c r="L12" s="93"/>
+      <c r="M12" s="85"/>
+      <c r="N12" s="85"/>
+      <c r="O12" s="87"/>
+      <c r="P12" s="87"/>
+      <c r="Q12" s="85"/>
+      <c r="R12" s="85"/>
+      <c r="S12" s="85"/>
+      <c r="T12" s="85"/>
+      <c r="U12" s="85"/>
+      <c r="V12" s="85"/>
+      <c r="W12" s="85"/>
+      <c r="X12" s="85"/>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A13" s="85"/>
+      <c r="B13" s="85"/>
+      <c r="C13" s="85"/>
+      <c r="D13" s="85"/>
+      <c r="E13" s="85"/>
+      <c r="F13" s="85"/>
+      <c r="G13" s="85"/>
+      <c r="H13" s="85"/>
+      <c r="I13" s="85"/>
+      <c r="J13" s="85"/>
+      <c r="K13" s="92"/>
+      <c r="L13" s="93"/>
+      <c r="M13" s="85"/>
+      <c r="N13" s="85"/>
+      <c r="O13" s="87"/>
+      <c r="P13" s="87"/>
+      <c r="Q13" s="85"/>
+      <c r="R13" s="85"/>
+      <c r="S13" s="85"/>
+      <c r="T13" s="85"/>
+      <c r="U13" s="85"/>
+      <c r="V13" s="85"/>
+      <c r="W13" s="85"/>
+      <c r="X13" s="85"/>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A14" s="85"/>
+      <c r="B14" s="85"/>
+      <c r="C14" s="85"/>
+      <c r="D14" s="85"/>
+      <c r="E14" s="85"/>
+      <c r="F14" s="85"/>
+      <c r="G14" s="85"/>
+      <c r="H14" s="85"/>
+      <c r="I14" s="85"/>
+      <c r="J14" s="85"/>
+      <c r="K14" s="92"/>
+      <c r="L14" s="93"/>
+      <c r="M14" s="85"/>
+      <c r="N14" s="85"/>
+      <c r="O14" s="87"/>
+      <c r="P14" s="87"/>
+      <c r="Q14" s="85"/>
+      <c r="R14" s="85"/>
+      <c r="S14" s="85"/>
+      <c r="T14" s="85"/>
+      <c r="U14" s="85"/>
+      <c r="V14" s="85"/>
+      <c r="W14" s="85"/>
+      <c r="X14" s="85"/>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A15" s="85"/>
+      <c r="B15" s="85"/>
+      <c r="C15" s="85"/>
+      <c r="D15" s="85"/>
+      <c r="E15" s="85"/>
+      <c r="F15" s="85"/>
+      <c r="G15" s="85"/>
+      <c r="H15" s="85"/>
+      <c r="I15" s="85"/>
+      <c r="J15" s="85"/>
+      <c r="K15" s="92"/>
+      <c r="L15" s="93"/>
+      <c r="M15" s="85"/>
+      <c r="N15" s="85"/>
+      <c r="O15" s="87"/>
+      <c r="P15" s="87"/>
+      <c r="Q15" s="85"/>
+      <c r="R15" s="85"/>
+      <c r="S15" s="85"/>
+      <c r="T15" s="85"/>
+      <c r="U15" s="85"/>
+      <c r="V15" s="85"/>
+      <c r="W15" s="85"/>
+      <c r="X15" s="85"/>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A16" s="85"/>
+      <c r="B16" s="85"/>
+      <c r="C16" s="85"/>
+      <c r="D16" s="85"/>
+      <c r="E16" s="85"/>
+      <c r="F16" s="85"/>
+      <c r="G16" s="85"/>
+      <c r="H16" s="85"/>
+      <c r="I16" s="85"/>
+      <c r="J16" s="85"/>
+      <c r="K16" s="92"/>
+      <c r="L16" s="93"/>
+      <c r="M16" s="85"/>
+      <c r="N16" s="85"/>
+      <c r="O16" s="87"/>
+      <c r="P16" s="87"/>
+      <c r="Q16" s="85"/>
+      <c r="R16" s="85"/>
+      <c r="S16" s="85"/>
+      <c r="T16" s="85"/>
+      <c r="U16" s="85"/>
+      <c r="V16" s="85"/>
+      <c r="W16" s="85"/>
+      <c r="X16" s="85"/>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A17" s="85"/>
+      <c r="B17" s="85"/>
+      <c r="C17" s="85"/>
+      <c r="D17" s="85"/>
+      <c r="E17" s="85"/>
+      <c r="F17" s="85"/>
+      <c r="G17" s="85"/>
+      <c r="H17" s="85"/>
+      <c r="I17" s="85"/>
+      <c r="J17" s="85"/>
+      <c r="K17" s="92"/>
+      <c r="L17" s="93"/>
+      <c r="M17" s="85"/>
+      <c r="N17" s="85"/>
+      <c r="O17" s="87"/>
+      <c r="P17" s="87"/>
+      <c r="Q17" s="85"/>
+      <c r="R17" s="85"/>
+      <c r="S17" s="85"/>
+      <c r="T17" s="85"/>
+      <c r="U17" s="85"/>
+      <c r="V17" s="85"/>
+      <c r="W17" s="85"/>
+      <c r="X17" s="85"/>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A18" s="85"/>
+      <c r="B18" s="85"/>
+      <c r="C18" s="85"/>
+      <c r="D18" s="85"/>
+      <c r="E18" s="85"/>
+      <c r="F18" s="85"/>
+      <c r="G18" s="85"/>
+      <c r="H18" s="85"/>
+      <c r="I18" s="85"/>
+      <c r="J18" s="85"/>
+      <c r="K18" s="92"/>
+      <c r="L18" s="93"/>
+      <c r="M18" s="85"/>
+      <c r="N18" s="85"/>
+      <c r="O18" s="87"/>
+      <c r="P18" s="87"/>
+      <c r="Q18" s="85"/>
+      <c r="R18" s="85"/>
+      <c r="S18" s="85"/>
+      <c r="T18" s="85"/>
+      <c r="U18" s="85"/>
+      <c r="V18" s="85"/>
+      <c r="W18" s="85"/>
+      <c r="X18" s="85"/>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A19" s="85"/>
+      <c r="B19" s="85"/>
+      <c r="C19" s="85"/>
+      <c r="D19" s="85"/>
+      <c r="E19" s="85"/>
+      <c r="F19" s="85"/>
+      <c r="G19" s="85"/>
+      <c r="H19" s="85"/>
+      <c r="I19" s="85"/>
+      <c r="J19" s="85"/>
+      <c r="K19" s="92"/>
+      <c r="L19" s="93"/>
+      <c r="M19" s="85"/>
+      <c r="N19" s="85"/>
+      <c r="O19" s="87"/>
+      <c r="P19" s="87"/>
+      <c r="Q19" s="85"/>
+      <c r="R19" s="85"/>
+      <c r="S19" s="85"/>
+      <c r="T19" s="85"/>
+      <c r="U19" s="85"/>
+      <c r="V19" s="85"/>
+      <c r="W19" s="85"/>
+      <c r="X19" s="85"/>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A20" s="85"/>
+      <c r="B20" s="85"/>
+      <c r="C20" s="85"/>
+      <c r="D20" s="85"/>
+      <c r="E20" s="85"/>
+      <c r="F20" s="85"/>
+      <c r="G20" s="85"/>
+      <c r="H20" s="85"/>
+      <c r="I20" s="85"/>
+      <c r="J20" s="85"/>
+      <c r="K20" s="92"/>
+      <c r="L20" s="93"/>
+      <c r="M20" s="85"/>
+      <c r="N20" s="85"/>
+      <c r="O20" s="87"/>
+      <c r="P20" s="87"/>
+      <c r="Q20" s="85"/>
+      <c r="R20" s="85"/>
+      <c r="S20" s="85"/>
+      <c r="T20" s="85"/>
+      <c r="U20" s="85"/>
+      <c r="V20" s="85"/>
+      <c r="W20" s="85"/>
+      <c r="X20" s="85"/>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A21" s="85"/>
+      <c r="B21" s="85"/>
+      <c r="C21" s="85"/>
+      <c r="D21" s="85"/>
+      <c r="E21" s="85"/>
+      <c r="F21" s="85"/>
+      <c r="G21" s="85"/>
+      <c r="H21" s="85"/>
+      <c r="I21" s="85"/>
+      <c r="J21" s="85"/>
+      <c r="K21" s="92"/>
+      <c r="L21" s="93"/>
+      <c r="M21" s="85"/>
+      <c r="N21" s="85"/>
+      <c r="O21" s="87"/>
+      <c r="P21" s="87"/>
+      <c r="Q21" s="85"/>
+      <c r="R21" s="85"/>
+      <c r="S21" s="85"/>
+      <c r="T21" s="85"/>
+      <c r="U21" s="85"/>
+      <c r="V21" s="85"/>
+      <c r="W21" s="85"/>
+      <c r="X21" s="85"/>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A22" s="85"/>
+      <c r="B22" s="85"/>
+      <c r="C22" s="85"/>
+      <c r="D22" s="85"/>
+      <c r="E22" s="85"/>
+      <c r="F22" s="85"/>
+      <c r="G22" s="85"/>
+      <c r="H22" s="85"/>
+      <c r="I22" s="85"/>
+      <c r="J22" s="85"/>
+      <c r="K22" s="92"/>
+      <c r="L22" s="93"/>
+      <c r="M22" s="85"/>
+      <c r="N22" s="85"/>
+      <c r="O22" s="87"/>
+      <c r="P22" s="87"/>
+      <c r="Q22" s="85"/>
+      <c r="R22" s="85"/>
+      <c r="S22" s="85"/>
+      <c r="T22" s="85"/>
+      <c r="U22" s="85"/>
+      <c r="V22" s="85"/>
+      <c r="W22" s="85"/>
+      <c r="X22" s="85"/>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A23" s="85"/>
+      <c r="B23" s="85"/>
+      <c r="C23" s="85"/>
+      <c r="D23" s="85"/>
+      <c r="E23" s="85"/>
+      <c r="F23" s="85"/>
+      <c r="G23" s="85"/>
+      <c r="H23" s="85"/>
+      <c r="I23" s="85"/>
+      <c r="J23" s="85"/>
+      <c r="K23" s="92"/>
+      <c r="L23" s="93"/>
+      <c r="M23" s="85"/>
+      <c r="N23" s="85"/>
+      <c r="O23" s="87"/>
+      <c r="P23" s="87"/>
+      <c r="Q23" s="85"/>
+      <c r="R23" s="85"/>
+      <c r="S23" s="85"/>
+      <c r="T23" s="85"/>
+      <c r="U23" s="85"/>
+      <c r="V23" s="85"/>
+      <c r="W23" s="85"/>
+      <c r="X23" s="85"/>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A24" s="85"/>
+      <c r="B24" s="85"/>
+      <c r="C24" s="85"/>
+      <c r="D24" s="85"/>
+      <c r="E24" s="85"/>
+      <c r="F24" s="85"/>
+      <c r="G24" s="85"/>
+      <c r="H24" s="85"/>
+      <c r="I24" s="85"/>
+      <c r="J24" s="85"/>
+      <c r="K24" s="92"/>
+      <c r="L24" s="93"/>
+      <c r="M24" s="85"/>
+      <c r="N24" s="85"/>
+      <c r="O24" s="87"/>
+      <c r="P24" s="87"/>
+      <c r="Q24" s="85"/>
+      <c r="R24" s="85"/>
+      <c r="S24" s="85"/>
+      <c r="T24" s="85"/>
+      <c r="U24" s="85"/>
+      <c r="V24" s="85"/>
+      <c r="W24" s="85"/>
+      <c r="X24" s="85"/>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A25" s="85"/>
+      <c r="B25" s="85"/>
+      <c r="C25" s="85"/>
+      <c r="D25" s="85"/>
+      <c r="E25" s="85"/>
+      <c r="F25" s="85"/>
+      <c r="G25" s="85"/>
+      <c r="H25" s="85"/>
+      <c r="I25" s="85"/>
+      <c r="J25" s="85"/>
+      <c r="K25" s="92"/>
+      <c r="L25" s="93"/>
+      <c r="M25" s="85"/>
+      <c r="N25" s="85"/>
+      <c r="O25" s="87"/>
+      <c r="P25" s="87"/>
+      <c r="Q25" s="85"/>
+      <c r="R25" s="85"/>
+      <c r="S25" s="85"/>
+      <c r="T25" s="85"/>
+      <c r="U25" s="85"/>
+      <c r="V25" s="85"/>
+      <c r="W25" s="85"/>
+      <c r="X25" s="85"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="R1:S1"/>
-    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="U1:V1"/>
+    <mergeCell ref="W1:X1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7:L7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="5" max="5" width="3.7109375" customWidth="1"/>
+    <col min="9" max="9" width="5.5703125" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" customWidth="1"/>
+    <col min="12" max="12" width="15.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="171" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="171"/>
+      <c r="C1" s="171"/>
+      <c r="D1" s="171"/>
+      <c r="E1" s="171"/>
+      <c r="F1" s="171"/>
+      <c r="G1" s="171"/>
+      <c r="H1" s="171"/>
+      <c r="I1" s="171"/>
+      <c r="J1" s="171"/>
+      <c r="K1" s="171"/>
+      <c r="L1" s="171"/>
+      <c r="M1" s="171"/>
+      <c r="N1" s="171"/>
+    </row>
+    <row r="2" spans="1:16" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="171"/>
+      <c r="B2" s="171"/>
+      <c r="C2" s="171"/>
+      <c r="D2" s="171"/>
+      <c r="E2" s="171"/>
+      <c r="F2" s="171"/>
+      <c r="G2" s="171"/>
+      <c r="H2" s="171"/>
+      <c r="I2" s="171"/>
+      <c r="J2" s="171"/>
+      <c r="K2" s="171"/>
+      <c r="L2" s="171"/>
+      <c r="M2" s="171"/>
+      <c r="N2" s="171"/>
+    </row>
+    <row r="3" spans="1:16" s="169" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="170"/>
+      <c r="B3" s="170"/>
+      <c r="C3" s="170"/>
+      <c r="D3" s="170"/>
+      <c r="E3" s="170"/>
+      <c r="F3" s="170"/>
+      <c r="G3" s="170"/>
+      <c r="H3" s="170"/>
+      <c r="I3" s="170"/>
+      <c r="J3" s="170"/>
+      <c r="K3" s="170"/>
+      <c r="L3" s="170"/>
+      <c r="M3" s="170"/>
+      <c r="N3" s="170"/>
+    </row>
+    <row r="4" spans="1:16" ht="55.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="177" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" s="172"/>
+      <c r="C4" s="172"/>
+      <c r="D4" s="123"/>
+      <c r="E4" s="123"/>
+      <c r="F4" s="184" t="s">
+        <v>77</v>
+      </c>
+      <c r="G4" s="184" t="s">
+        <v>82</v>
+      </c>
+      <c r="H4" s="185" t="s">
+        <v>83</v>
+      </c>
+      <c r="I4" s="185"/>
+      <c r="J4" s="185"/>
+      <c r="K4" s="186" t="s">
+        <v>84</v>
+      </c>
+      <c r="L4" s="187" t="s">
+        <v>85</v>
+      </c>
+      <c r="M4" s="188" t="s">
+        <v>86</v>
+      </c>
+      <c r="N4" s="188" t="s">
+        <v>34</v>
+      </c>
+      <c r="P4" s="143"/>
+    </row>
+    <row r="5" spans="1:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="178" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" s="124"/>
+      <c r="C5" s="124" t="s">
+        <v>88</v>
+      </c>
+      <c r="D5" s="125"/>
+      <c r="E5" s="125"/>
+      <c r="F5" s="126"/>
+      <c r="G5" s="127"/>
+      <c r="H5" s="145"/>
+      <c r="I5" s="144"/>
+      <c r="J5" s="128"/>
+      <c r="K5" s="127"/>
+      <c r="L5" s="129"/>
+      <c r="M5" s="130"/>
+      <c r="N5" s="131"/>
+    </row>
+    <row r="6" spans="1:16" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="179"/>
+      <c r="B6" s="140"/>
+      <c r="C6" s="142" t="s">
+        <v>89</v>
+      </c>
+      <c r="D6" s="141"/>
+      <c r="E6" s="139"/>
+      <c r="F6" s="189" t="s">
+        <v>90</v>
+      </c>
+      <c r="G6" s="184" t="s">
+        <v>91</v>
+      </c>
+      <c r="H6" s="190" t="s">
+        <v>92</v>
+      </c>
+      <c r="I6" s="191"/>
+      <c r="J6" s="191"/>
+      <c r="K6" s="191"/>
+      <c r="L6" s="192"/>
+      <c r="M6" s="193" t="s">
+        <v>35</v>
+      </c>
+      <c r="N6" s="194"/>
+    </row>
+    <row r="7" spans="1:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="180" t="s">
+        <v>93</v>
+      </c>
+      <c r="B7" s="181" t="s">
+        <v>94</v>
+      </c>
+      <c r="C7" s="182" t="s">
+        <v>67</v>
+      </c>
+      <c r="D7" s="183" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" s="147"/>
+      <c r="F7" s="156"/>
+      <c r="G7" s="132"/>
+      <c r="H7" s="145"/>
+      <c r="I7" s="144"/>
+      <c r="J7" s="144"/>
+      <c r="K7" s="144"/>
+      <c r="L7" s="173"/>
+      <c r="M7" s="157"/>
+      <c r="N7" s="157"/>
+    </row>
+    <row r="8" spans="1:16" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="158"/>
+      <c r="B8" s="158"/>
+      <c r="C8" s="159"/>
+      <c r="D8" s="159"/>
+      <c r="E8" s="147"/>
+      <c r="F8" s="150"/>
+      <c r="G8" s="151"/>
+      <c r="H8" s="152"/>
+      <c r="I8" s="152"/>
+      <c r="J8" s="153"/>
+      <c r="K8" s="154"/>
+      <c r="L8" s="154"/>
+      <c r="M8" s="155"/>
+      <c r="N8" s="155"/>
+    </row>
+    <row r="9" spans="1:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="160"/>
+      <c r="B9" s="161"/>
+      <c r="C9" s="162"/>
+      <c r="D9" s="163"/>
+      <c r="E9" s="148"/>
+      <c r="F9" s="195" t="s">
+        <v>0</v>
+      </c>
+      <c r="G9" s="196"/>
+      <c r="H9" s="196"/>
+      <c r="I9" s="196"/>
+      <c r="J9" s="196"/>
+      <c r="K9" s="197"/>
+      <c r="L9" s="195" t="s">
+        <v>95</v>
+      </c>
+      <c r="M9" s="196"/>
+      <c r="N9" s="197"/>
+    </row>
+    <row r="10" spans="1:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="160"/>
+      <c r="B10" s="161"/>
+      <c r="C10" s="164"/>
+      <c r="D10" s="165"/>
+      <c r="E10" s="148"/>
+      <c r="F10" s="174"/>
+      <c r="G10" s="133"/>
+      <c r="H10" s="133"/>
+      <c r="I10" s="133"/>
+      <c r="J10" s="133"/>
+      <c r="K10" s="134"/>
+      <c r="L10" s="174"/>
+      <c r="M10" s="133"/>
+      <c r="N10" s="134"/>
+    </row>
+    <row r="11" spans="1:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="160"/>
+      <c r="B11" s="161"/>
+      <c r="C11" s="164"/>
+      <c r="D11" s="165"/>
+      <c r="E11" s="148"/>
+      <c r="F11" s="175"/>
+      <c r="G11" s="135"/>
+      <c r="H11" s="135"/>
+      <c r="I11" s="135"/>
+      <c r="J11" s="135"/>
+      <c r="K11" s="136"/>
+      <c r="L11" s="175"/>
+      <c r="M11" s="135"/>
+      <c r="N11" s="136"/>
+    </row>
+    <row r="12" spans="1:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="160"/>
+      <c r="B12" s="161"/>
+      <c r="C12" s="164"/>
+      <c r="D12" s="165"/>
+      <c r="E12" s="148"/>
+      <c r="F12" s="175"/>
+      <c r="G12" s="135"/>
+      <c r="H12" s="135"/>
+      <c r="I12" s="135"/>
+      <c r="J12" s="135"/>
+      <c r="K12" s="136"/>
+      <c r="L12" s="175"/>
+      <c r="M12" s="135"/>
+      <c r="N12" s="136"/>
+    </row>
+    <row r="13" spans="1:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="160"/>
+      <c r="B13" s="161"/>
+      <c r="C13" s="162"/>
+      <c r="D13" s="163"/>
+      <c r="E13" s="148"/>
+      <c r="F13" s="175"/>
+      <c r="G13" s="135"/>
+      <c r="H13" s="135"/>
+      <c r="I13" s="135"/>
+      <c r="J13" s="135"/>
+      <c r="K13" s="136"/>
+      <c r="L13" s="175"/>
+      <c r="M13" s="135"/>
+      <c r="N13" s="136"/>
+    </row>
+    <row r="14" spans="1:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="160"/>
+      <c r="B14" s="161"/>
+      <c r="C14" s="162"/>
+      <c r="D14" s="163"/>
+      <c r="E14" s="148"/>
+      <c r="F14" s="175"/>
+      <c r="G14" s="135"/>
+      <c r="H14" s="135"/>
+      <c r="I14" s="135"/>
+      <c r="J14" s="135"/>
+      <c r="K14" s="136"/>
+      <c r="L14" s="175"/>
+      <c r="M14" s="135"/>
+      <c r="N14" s="136"/>
+    </row>
+    <row r="15" spans="1:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="160"/>
+      <c r="B15" s="161"/>
+      <c r="C15" s="162"/>
+      <c r="D15" s="163"/>
+      <c r="E15" s="148"/>
+      <c r="F15" s="175"/>
+      <c r="G15" s="135"/>
+      <c r="H15" s="135"/>
+      <c r="I15" s="135"/>
+      <c r="J15" s="135"/>
+      <c r="K15" s="136"/>
+      <c r="L15" s="175"/>
+      <c r="M15" s="135"/>
+      <c r="N15" s="136"/>
+    </row>
+    <row r="16" spans="1:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="160"/>
+      <c r="B16" s="161"/>
+      <c r="C16" s="162"/>
+      <c r="D16" s="163"/>
+      <c r="E16" s="148"/>
+      <c r="F16" s="175"/>
+      <c r="G16" s="135"/>
+      <c r="H16" s="135"/>
+      <c r="I16" s="135"/>
+      <c r="J16" s="135"/>
+      <c r="K16" s="136"/>
+      <c r="L16" s="175"/>
+      <c r="M16" s="135"/>
+      <c r="N16" s="136"/>
+    </row>
+    <row r="17" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="160"/>
+      <c r="B17" s="161"/>
+      <c r="C17" s="162"/>
+      <c r="D17" s="163"/>
+      <c r="E17" s="148"/>
+      <c r="F17" s="175"/>
+      <c r="G17" s="135"/>
+      <c r="H17" s="135"/>
+      <c r="I17" s="135"/>
+      <c r="J17" s="135"/>
+      <c r="K17" s="136"/>
+      <c r="L17" s="175"/>
+      <c r="M17" s="135"/>
+      <c r="N17" s="136"/>
+    </row>
+    <row r="18" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="166"/>
+      <c r="B18" s="161"/>
+      <c r="C18" s="162"/>
+      <c r="D18" s="163"/>
+      <c r="E18" s="148"/>
+      <c r="F18" s="175"/>
+      <c r="G18" s="135"/>
+      <c r="H18" s="135"/>
+      <c r="I18" s="135"/>
+      <c r="J18" s="135"/>
+      <c r="K18" s="136"/>
+      <c r="L18" s="175"/>
+      <c r="M18" s="135"/>
+      <c r="N18" s="136"/>
+    </row>
+    <row r="19" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="160" t="s">
+        <v>96</v>
+      </c>
+      <c r="B19" s="161" t="s">
+        <v>96</v>
+      </c>
+      <c r="C19" s="162"/>
+      <c r="D19" s="163"/>
+      <c r="E19" s="148"/>
+      <c r="F19" s="175"/>
+      <c r="G19" s="135"/>
+      <c r="H19" s="135"/>
+      <c r="I19" s="135"/>
+      <c r="J19" s="135"/>
+      <c r="K19" s="136"/>
+      <c r="L19" s="175"/>
+      <c r="M19" s="135"/>
+      <c r="N19" s="136"/>
+    </row>
+    <row r="20" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="167"/>
+      <c r="B20" s="168"/>
+      <c r="C20" s="162"/>
+      <c r="D20" s="163"/>
+      <c r="E20" s="148"/>
+      <c r="F20" s="176"/>
+      <c r="G20" s="137"/>
+      <c r="H20" s="137"/>
+      <c r="I20" s="137"/>
+      <c r="J20" s="137"/>
+      <c r="K20" s="138"/>
+      <c r="L20" s="176"/>
+      <c r="M20" s="137"/>
+      <c r="N20" s="138"/>
+    </row>
+    <row r="21" spans="1:14" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C21" s="198" t="s">
+        <v>97</v>
+      </c>
+      <c r="D21" s="149"/>
+      <c r="E21" s="146"/>
+    </row>
+  </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="L10:N20"/>
+    <mergeCell ref="F10:K20"/>
+    <mergeCell ref="F9:K9"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H6:L6"/>
+    <mergeCell ref="H7:L7"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="A1:N2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
reporte detallereceta (agregar ingredientes , instrucciones y foto)
</commit_message>
<xml_diff>
--- a/ExcelAddIn1/Resources/FICHA RECETA.xlsx
+++ b/ExcelAddIn1/Resources/FICHA RECETA.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MANOLO\Desktop\JOB\proyecto cocina\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MANOLO\Documents\GitHub\VSTOexcelRest\ExcelAddIn1\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19560" windowHeight="8340" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19560" windowHeight="8340" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ReporteInventario" sheetId="3" r:id="rId1"/>
@@ -1604,6 +1604,9 @@
     <xf numFmtId="0" fontId="4" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -1788,17 +1791,14 @@
     <xf numFmtId="0" fontId="17" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="13" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2396,45 +2396,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="147" t="s">
+      <c r="B1" s="148" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="147"/>
-      <c r="D1" s="147"/>
-      <c r="E1" s="147"/>
-      <c r="F1" s="147"/>
+      <c r="C1" s="148"/>
+      <c r="D1" s="148"/>
+      <c r="E1" s="148"/>
+      <c r="F1" s="148"/>
       <c r="G1" s="66" t="s">
         <v>54</v>
       </c>
       <c r="H1" s="66"/>
-      <c r="I1" s="148">
+      <c r="I1" s="149">
         <v>42491</v>
       </c>
-      <c r="J1" s="148"/>
+      <c r="J1" s="149"/>
     </row>
     <row r="2" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="147"/>
-      <c r="C2" s="147"/>
-      <c r="D2" s="147"/>
-      <c r="E2" s="147"/>
-      <c r="F2" s="147"/>
+      <c r="B2" s="148"/>
+      <c r="C2" s="148"/>
+      <c r="D2" s="148"/>
+      <c r="E2" s="148"/>
+      <c r="F2" s="148"/>
       <c r="G2" s="68" t="s">
         <v>55</v>
       </c>
       <c r="H2" s="68"/>
-      <c r="I2" s="148">
+      <c r="I2" s="149">
         <v>42639</v>
       </c>
-      <c r="J2" s="148"/>
+      <c r="J2" s="149"/>
     </row>
     <row r="3" spans="1:10" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="146" t="s">
+      <c r="B3" s="147" t="s">
         <v>56</v>
       </c>
-      <c r="C3" s="146"/>
-      <c r="D3" s="146"/>
-      <c r="E3" s="146"/>
-      <c r="F3" s="146"/>
+      <c r="C3" s="147"/>
+      <c r="D3" s="147"/>
+      <c r="E3" s="147"/>
+      <c r="F3" s="147"/>
       <c r="G3" s="67"/>
       <c r="H3" s="67"/>
       <c r="I3" s="65"/>
@@ -2592,52 +2592,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="168" t="s">
+      <c r="A1" s="169" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="159" t="s">
+      <c r="B1" s="160" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="160"/>
-      <c r="D1" s="160"/>
-      <c r="E1" s="160"/>
-      <c r="F1" s="161"/>
+      <c r="C1" s="161"/>
+      <c r="D1" s="161"/>
+      <c r="E1" s="161"/>
+      <c r="F1" s="162"/>
       <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="169"/>
-      <c r="B2" s="162" t="s">
+      <c r="A2" s="170"/>
+      <c r="B2" s="163" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="163"/>
-      <c r="D2" s="163"/>
-      <c r="E2" s="163"/>
-      <c r="F2" s="164"/>
-      <c r="G2" s="151" t="s">
+      <c r="C2" s="164"/>
+      <c r="D2" s="164"/>
+      <c r="E2" s="164"/>
+      <c r="F2" s="165"/>
+      <c r="G2" s="152" t="s">
         <v>47</v>
       </c>
-      <c r="H2" s="155" t="s">
+      <c r="H2" s="156" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="156"/>
+      <c r="I2" s="157"/>
       <c r="J2" s="19">
         <v>0.85</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="170"/>
-      <c r="B3" s="165"/>
-      <c r="C3" s="166"/>
-      <c r="D3" s="166"/>
-      <c r="E3" s="166"/>
-      <c r="F3" s="167"/>
-      <c r="G3" s="152"/>
-      <c r="H3" s="155" t="s">
+      <c r="A3" s="171"/>
+      <c r="B3" s="166"/>
+      <c r="C3" s="167"/>
+      <c r="D3" s="167"/>
+      <c r="E3" s="167"/>
+      <c r="F3" s="168"/>
+      <c r="G3" s="153"/>
+      <c r="H3" s="156" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="156"/>
+      <c r="I3" s="157"/>
       <c r="J3" s="20">
         <v>10</v>
       </c>
@@ -2664,10 +2664,10 @@
       <c r="G4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="157" t="s">
+      <c r="H4" s="158" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="158"/>
+      <c r="I4" s="159"/>
       <c r="J4" s="23">
         <v>8.5</v>
       </c>
@@ -2680,10 +2680,10 @@
       <c r="E5" s="24"/>
       <c r="F5" s="26"/>
       <c r="G5" s="26"/>
-      <c r="H5" s="153" t="s">
+      <c r="H5" s="154" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="154"/>
+      <c r="I5" s="155"/>
       <c r="J5" s="27">
         <f>SUM(G5:G100)</f>
         <v>0</v>
@@ -2697,10 +2697,10 @@
       <c r="E6" s="24"/>
       <c r="F6" s="26"/>
       <c r="G6" s="26"/>
-      <c r="H6" s="153" t="s">
+      <c r="H6" s="154" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="154"/>
+      <c r="I6" s="155"/>
       <c r="J6" s="28">
         <f>J5*0.05</f>
         <v>0</v>
@@ -2714,10 +2714,10 @@
       <c r="E7" s="24"/>
       <c r="F7" s="26"/>
       <c r="G7" s="26"/>
-      <c r="H7" s="153" t="s">
+      <c r="H7" s="154" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="154"/>
+      <c r="I7" s="155"/>
       <c r="J7" s="28">
         <v>110</v>
       </c>
@@ -2730,10 +2730,10 @@
       <c r="E8" s="24"/>
       <c r="F8" s="26"/>
       <c r="G8" s="26"/>
-      <c r="H8" s="153" t="s">
+      <c r="H8" s="154" t="s">
         <v>14</v>
       </c>
-      <c r="I8" s="154"/>
+      <c r="I8" s="155"/>
       <c r="J8" s="29">
         <v>150</v>
       </c>
@@ -2746,10 +2746,10 @@
       <c r="E9" s="24"/>
       <c r="F9" s="26"/>
       <c r="G9" s="26"/>
-      <c r="H9" s="153" t="s">
+      <c r="H9" s="154" t="s">
         <v>15</v>
       </c>
-      <c r="I9" s="153"/>
+      <c r="I9" s="154"/>
       <c r="J9" s="30">
         <f>(PRECIO_VENTA*LITROS_A_ELABORAR)</f>
         <v>1500</v>
@@ -2763,10 +2763,10 @@
       <c r="E10" s="24"/>
       <c r="F10" s="26"/>
       <c r="G10" s="26"/>
-      <c r="H10" s="153" t="s">
+      <c r="H10" s="154" t="s">
         <v>16</v>
       </c>
-      <c r="I10" s="153"/>
+      <c r="I10" s="154"/>
       <c r="J10" s="31">
         <f>J9-COSTO_TOTAL_MATERIA_PRIMA</f>
         <v>1500</v>
@@ -2780,10 +2780,10 @@
       <c r="E11" s="24"/>
       <c r="F11" s="26"/>
       <c r="G11" s="26"/>
-      <c r="H11" s="149" t="s">
+      <c r="H11" s="150" t="s">
         <v>19</v>
       </c>
-      <c r="I11" s="150"/>
+      <c r="I11" s="151"/>
       <c r="J11" s="32">
         <v>0.27</v>
       </c>
@@ -2796,10 +2796,10 @@
       <c r="E12" s="24"/>
       <c r="F12" s="26"/>
       <c r="G12" s="26"/>
-      <c r="H12" s="149" t="s">
+      <c r="H12" s="150" t="s">
         <v>20</v>
       </c>
-      <c r="I12" s="150"/>
+      <c r="I12" s="151"/>
       <c r="J12" s="32">
         <f>((J5+COSTO_PREPARACION)/J9-1)*(-1)</f>
         <v>0.92666666666666664</v>
@@ -2939,22 +2939,22 @@
       <c r="N1" s="81"/>
       <c r="O1" s="81"/>
       <c r="P1" s="81"/>
-      <c r="Q1" s="171" t="s">
+      <c r="Q1" s="172" t="s">
         <v>60</v>
       </c>
-      <c r="R1" s="172"/>
-      <c r="S1" s="171" t="s">
+      <c r="R1" s="173"/>
+      <c r="S1" s="172" t="s">
         <v>61</v>
       </c>
-      <c r="T1" s="172"/>
-      <c r="U1" s="171" t="s">
+      <c r="T1" s="173"/>
+      <c r="U1" s="172" t="s">
         <v>62</v>
       </c>
-      <c r="V1" s="172"/>
-      <c r="W1" s="171" t="s">
+      <c r="V1" s="173"/>
+      <c r="W1" s="172" t="s">
         <v>63</v>
       </c>
-      <c r="X1" s="172"/>
+      <c r="X1" s="173"/>
       <c r="Y1" s="81"/>
       <c r="Z1" s="81"/>
       <c r="AA1" s="81"/>
@@ -3654,8 +3654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7:N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3670,36 +3670,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="198"/>
-      <c r="B1" s="198"/>
-      <c r="C1" s="198"/>
-      <c r="D1" s="198"/>
-      <c r="E1" s="198"/>
-      <c r="F1" s="198"/>
-      <c r="G1" s="198"/>
-      <c r="H1" s="198"/>
-      <c r="I1" s="198"/>
-      <c r="J1" s="198"/>
-      <c r="K1" s="198"/>
-      <c r="L1" s="198"/>
-      <c r="M1" s="198"/>
-      <c r="N1" s="198"/>
+      <c r="A1" s="199"/>
+      <c r="B1" s="199"/>
+      <c r="C1" s="199"/>
+      <c r="D1" s="199"/>
+      <c r="E1" s="199"/>
+      <c r="F1" s="199"/>
+      <c r="G1" s="199"/>
+      <c r="H1" s="199"/>
+      <c r="I1" s="199"/>
+      <c r="J1" s="199"/>
+      <c r="K1" s="199"/>
+      <c r="L1" s="199"/>
+      <c r="M1" s="199"/>
+      <c r="N1" s="199"/>
     </row>
     <row r="2" spans="1:16" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="198"/>
-      <c r="B2" s="198"/>
-      <c r="C2" s="198"/>
-      <c r="D2" s="198"/>
-      <c r="E2" s="198"/>
-      <c r="F2" s="198"/>
-      <c r="G2" s="198"/>
-      <c r="H2" s="198"/>
-      <c r="I2" s="198"/>
-      <c r="J2" s="198"/>
-      <c r="K2" s="198"/>
-      <c r="L2" s="198"/>
-      <c r="M2" s="198"/>
-      <c r="N2" s="198"/>
+      <c r="A2" s="199"/>
+      <c r="B2" s="199"/>
+      <c r="C2" s="199"/>
+      <c r="D2" s="199"/>
+      <c r="E2" s="199"/>
+      <c r="F2" s="199"/>
+      <c r="G2" s="199"/>
+      <c r="H2" s="199"/>
+      <c r="I2" s="199"/>
+      <c r="J2" s="199"/>
+      <c r="K2" s="199"/>
+      <c r="L2" s="199"/>
+      <c r="M2" s="199"/>
+      <c r="N2" s="199"/>
     </row>
     <row r="3" spans="1:16" s="133" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="134"/>
@@ -3721,8 +3721,8 @@
       <c r="A4" s="135" t="s">
         <v>80</v>
       </c>
-      <c r="B4" s="192"/>
-      <c r="C4" s="192"/>
+      <c r="B4" s="193"/>
+      <c r="C4" s="193"/>
       <c r="D4" s="96"/>
       <c r="E4" s="96"/>
       <c r="F4" s="140" t="s">
@@ -3731,11 +3731,11 @@
       <c r="G4" s="140" t="s">
         <v>81</v>
       </c>
-      <c r="H4" s="185" t="s">
+      <c r="H4" s="186" t="s">
         <v>82</v>
       </c>
-      <c r="I4" s="185"/>
-      <c r="J4" s="185"/>
+      <c r="I4" s="186"/>
+      <c r="J4" s="186"/>
       <c r="K4" s="141" t="s">
         <v>83</v>
       </c>
@@ -3751,7 +3751,7 @@
       <c r="P4" s="110"/>
     </row>
     <row r="5" spans="1:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="193" t="s">
+      <c r="A5" s="194" t="s">
         <v>86</v>
       </c>
       <c r="B5" s="97"/>
@@ -3762,8 +3762,8 @@
       <c r="E5" s="98"/>
       <c r="F5" s="99"/>
       <c r="G5" s="100"/>
-      <c r="H5" s="186"/>
-      <c r="I5" s="187"/>
+      <c r="H5" s="187"/>
+      <c r="I5" s="188"/>
       <c r="J5" s="101"/>
       <c r="K5" s="100"/>
       <c r="L5" s="102"/>
@@ -3771,7 +3771,7 @@
       <c r="N5" s="104"/>
     </row>
     <row r="6" spans="1:16" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="194"/>
+      <c r="A6" s="195"/>
       <c r="B6" s="107"/>
       <c r="C6" s="109" t="s">
         <v>88</v>
@@ -3784,17 +3784,17 @@
       <c r="G6" s="140" t="s">
         <v>90</v>
       </c>
-      <c r="H6" s="188" t="s">
+      <c r="H6" s="189" t="s">
         <v>91</v>
       </c>
-      <c r="I6" s="189"/>
-      <c r="J6" s="189"/>
-      <c r="K6" s="189"/>
-      <c r="L6" s="190"/>
-      <c r="M6" s="195" t="s">
+      <c r="I6" s="190"/>
+      <c r="J6" s="190"/>
+      <c r="K6" s="190"/>
+      <c r="L6" s="191"/>
+      <c r="M6" s="196" t="s">
         <v>35</v>
       </c>
-      <c r="N6" s="196"/>
+      <c r="N6" s="197"/>
     </row>
     <row r="7" spans="1:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="136" t="s">
@@ -3812,13 +3812,13 @@
       <c r="E7" s="112"/>
       <c r="F7" s="121"/>
       <c r="G7" s="105"/>
-      <c r="H7" s="186"/>
-      <c r="I7" s="187"/>
-      <c r="J7" s="187"/>
-      <c r="K7" s="187"/>
-      <c r="L7" s="191"/>
-      <c r="M7" s="197"/>
-      <c r="N7" s="197"/>
+      <c r="H7" s="187"/>
+      <c r="I7" s="188"/>
+      <c r="J7" s="188"/>
+      <c r="K7" s="188"/>
+      <c r="L7" s="192"/>
+      <c r="M7" s="198"/>
+      <c r="N7" s="198"/>
     </row>
     <row r="8" spans="1:16" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="122"/>
@@ -3842,19 +3842,19 @@
       <c r="C9" s="126"/>
       <c r="D9" s="127"/>
       <c r="E9" s="113"/>
-      <c r="F9" s="182" t="s">
+      <c r="F9" s="183" t="s">
         <v>0</v>
       </c>
-      <c r="G9" s="183"/>
-      <c r="H9" s="183"/>
-      <c r="I9" s="183"/>
-      <c r="J9" s="183"/>
-      <c r="K9" s="184"/>
-      <c r="L9" s="182" t="s">
+      <c r="G9" s="184"/>
+      <c r="H9" s="184"/>
+      <c r="I9" s="184"/>
+      <c r="J9" s="184"/>
+      <c r="K9" s="185"/>
+      <c r="L9" s="183" t="s">
         <v>94</v>
       </c>
-      <c r="M9" s="183"/>
-      <c r="N9" s="184"/>
+      <c r="M9" s="184"/>
+      <c r="N9" s="185"/>
     </row>
     <row r="10" spans="1:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="124"/>
@@ -3862,15 +3862,15 @@
       <c r="C10" s="128"/>
       <c r="D10" s="129"/>
       <c r="E10" s="113"/>
-      <c r="F10" s="173"/>
-      <c r="G10" s="174"/>
-      <c r="H10" s="174"/>
-      <c r="I10" s="174"/>
-      <c r="J10" s="174"/>
-      <c r="K10" s="175"/>
-      <c r="L10" s="173"/>
-      <c r="M10" s="174"/>
-      <c r="N10" s="175"/>
+      <c r="F10" s="174"/>
+      <c r="G10" s="175"/>
+      <c r="H10" s="175"/>
+      <c r="I10" s="175"/>
+      <c r="J10" s="175"/>
+      <c r="K10" s="176"/>
+      <c r="L10" s="174"/>
+      <c r="M10" s="175"/>
+      <c r="N10" s="176"/>
     </row>
     <row r="11" spans="1:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="124"/>
@@ -3878,15 +3878,15 @@
       <c r="C11" s="128"/>
       <c r="D11" s="129"/>
       <c r="E11" s="113"/>
-      <c r="F11" s="176"/>
-      <c r="G11" s="177"/>
-      <c r="H11" s="177"/>
-      <c r="I11" s="177"/>
-      <c r="J11" s="177"/>
-      <c r="K11" s="178"/>
-      <c r="L11" s="176"/>
-      <c r="M11" s="177"/>
-      <c r="N11" s="178"/>
+      <c r="F11" s="177"/>
+      <c r="G11" s="178"/>
+      <c r="H11" s="178"/>
+      <c r="I11" s="178"/>
+      <c r="J11" s="178"/>
+      <c r="K11" s="179"/>
+      <c r="L11" s="177"/>
+      <c r="M11" s="178"/>
+      <c r="N11" s="179"/>
     </row>
     <row r="12" spans="1:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="124"/>
@@ -3894,15 +3894,15 @@
       <c r="C12" s="128"/>
       <c r="D12" s="129"/>
       <c r="E12" s="113"/>
-      <c r="F12" s="176"/>
-      <c r="G12" s="177"/>
-      <c r="H12" s="177"/>
-      <c r="I12" s="177"/>
-      <c r="J12" s="177"/>
-      <c r="K12" s="178"/>
-      <c r="L12" s="176"/>
-      <c r="M12" s="177"/>
-      <c r="N12" s="178"/>
+      <c r="F12" s="177"/>
+      <c r="G12" s="178"/>
+      <c r="H12" s="178"/>
+      <c r="I12" s="178"/>
+      <c r="J12" s="178"/>
+      <c r="K12" s="179"/>
+      <c r="L12" s="177"/>
+      <c r="M12" s="178"/>
+      <c r="N12" s="179"/>
     </row>
     <row r="13" spans="1:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="124"/>
@@ -3910,15 +3910,15 @@
       <c r="C13" s="126"/>
       <c r="D13" s="127"/>
       <c r="E13" s="113"/>
-      <c r="F13" s="176"/>
-      <c r="G13" s="177"/>
-      <c r="H13" s="177"/>
-      <c r="I13" s="177"/>
-      <c r="J13" s="177"/>
-      <c r="K13" s="178"/>
-      <c r="L13" s="176"/>
-      <c r="M13" s="177"/>
-      <c r="N13" s="178"/>
+      <c r="F13" s="177"/>
+      <c r="G13" s="178"/>
+      <c r="H13" s="178"/>
+      <c r="I13" s="178"/>
+      <c r="J13" s="178"/>
+      <c r="K13" s="179"/>
+      <c r="L13" s="177"/>
+      <c r="M13" s="178"/>
+      <c r="N13" s="179"/>
     </row>
     <row r="14" spans="1:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="124"/>
@@ -3926,15 +3926,15 @@
       <c r="C14" s="126"/>
       <c r="D14" s="127"/>
       <c r="E14" s="113"/>
-      <c r="F14" s="176"/>
-      <c r="G14" s="177"/>
-      <c r="H14" s="177"/>
-      <c r="I14" s="177"/>
-      <c r="J14" s="177"/>
-      <c r="K14" s="178"/>
-      <c r="L14" s="176"/>
-      <c r="M14" s="177"/>
-      <c r="N14" s="178"/>
+      <c r="F14" s="177"/>
+      <c r="G14" s="178"/>
+      <c r="H14" s="178"/>
+      <c r="I14" s="178"/>
+      <c r="J14" s="178"/>
+      <c r="K14" s="179"/>
+      <c r="L14" s="177"/>
+      <c r="M14" s="178"/>
+      <c r="N14" s="179"/>
     </row>
     <row r="15" spans="1:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="124"/>
@@ -3942,15 +3942,15 @@
       <c r="C15" s="126"/>
       <c r="D15" s="127"/>
       <c r="E15" s="113"/>
-      <c r="F15" s="176"/>
-      <c r="G15" s="177"/>
-      <c r="H15" s="177"/>
-      <c r="I15" s="177"/>
-      <c r="J15" s="177"/>
-      <c r="K15" s="178"/>
-      <c r="L15" s="176"/>
-      <c r="M15" s="177"/>
-      <c r="N15" s="178"/>
+      <c r="F15" s="177"/>
+      <c r="G15" s="178"/>
+      <c r="H15" s="178"/>
+      <c r="I15" s="178"/>
+      <c r="J15" s="178"/>
+      <c r="K15" s="179"/>
+      <c r="L15" s="177"/>
+      <c r="M15" s="178"/>
+      <c r="N15" s="179"/>
     </row>
     <row r="16" spans="1:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="124"/>
@@ -3958,15 +3958,15 @@
       <c r="C16" s="126"/>
       <c r="D16" s="127"/>
       <c r="E16" s="113"/>
-      <c r="F16" s="176"/>
-      <c r="G16" s="177"/>
-      <c r="H16" s="177"/>
-      <c r="I16" s="177"/>
-      <c r="J16" s="177"/>
-      <c r="K16" s="178"/>
-      <c r="L16" s="176"/>
-      <c r="M16" s="177"/>
-      <c r="N16" s="178"/>
+      <c r="F16" s="177"/>
+      <c r="G16" s="178"/>
+      <c r="H16" s="178"/>
+      <c r="I16" s="178"/>
+      <c r="J16" s="178"/>
+      <c r="K16" s="179"/>
+      <c r="L16" s="177"/>
+      <c r="M16" s="178"/>
+      <c r="N16" s="179"/>
     </row>
     <row r="17" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="124"/>
@@ -3974,15 +3974,15 @@
       <c r="C17" s="126"/>
       <c r="D17" s="127"/>
       <c r="E17" s="113"/>
-      <c r="F17" s="176"/>
-      <c r="G17" s="177"/>
-      <c r="H17" s="177"/>
-      <c r="I17" s="177"/>
-      <c r="J17" s="177"/>
-      <c r="K17" s="178"/>
-      <c r="L17" s="176"/>
-      <c r="M17" s="177"/>
-      <c r="N17" s="178"/>
+      <c r="F17" s="177"/>
+      <c r="G17" s="178"/>
+      <c r="H17" s="178"/>
+      <c r="I17" s="178"/>
+      <c r="J17" s="178"/>
+      <c r="K17" s="179"/>
+      <c r="L17" s="177"/>
+      <c r="M17" s="178"/>
+      <c r="N17" s="179"/>
     </row>
     <row r="18" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="130"/>
@@ -3990,15 +3990,15 @@
       <c r="C18" s="126"/>
       <c r="D18" s="127"/>
       <c r="E18" s="113"/>
-      <c r="F18" s="176"/>
-      <c r="G18" s="177"/>
-      <c r="H18" s="177"/>
-      <c r="I18" s="177"/>
-      <c r="J18" s="177"/>
-      <c r="K18" s="178"/>
-      <c r="L18" s="176"/>
-      <c r="M18" s="177"/>
-      <c r="N18" s="178"/>
+      <c r="F18" s="177"/>
+      <c r="G18" s="178"/>
+      <c r="H18" s="178"/>
+      <c r="I18" s="178"/>
+      <c r="J18" s="178"/>
+      <c r="K18" s="179"/>
+      <c r="L18" s="177"/>
+      <c r="M18" s="178"/>
+      <c r="N18" s="179"/>
     </row>
     <row r="19" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="124" t="s">
@@ -4010,15 +4010,15 @@
       <c r="C19" s="126"/>
       <c r="D19" s="127"/>
       <c r="E19" s="113"/>
-      <c r="F19" s="176"/>
-      <c r="G19" s="177"/>
-      <c r="H19" s="177"/>
-      <c r="I19" s="177"/>
-      <c r="J19" s="177"/>
-      <c r="K19" s="178"/>
-      <c r="L19" s="176"/>
-      <c r="M19" s="177"/>
-      <c r="N19" s="178"/>
+      <c r="F19" s="177"/>
+      <c r="G19" s="178"/>
+      <c r="H19" s="178"/>
+      <c r="I19" s="178"/>
+      <c r="J19" s="178"/>
+      <c r="K19" s="179"/>
+      <c r="L19" s="177"/>
+      <c r="M19" s="178"/>
+      <c r="N19" s="179"/>
     </row>
     <row r="20" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="131"/>
@@ -4026,15 +4026,15 @@
       <c r="C20" s="126"/>
       <c r="D20" s="127"/>
       <c r="E20" s="113"/>
-      <c r="F20" s="179"/>
-      <c r="G20" s="180"/>
-      <c r="H20" s="180"/>
-      <c r="I20" s="180"/>
-      <c r="J20" s="180"/>
-      <c r="K20" s="181"/>
-      <c r="L20" s="179"/>
-      <c r="M20" s="180"/>
-      <c r="N20" s="181"/>
+      <c r="F20" s="180"/>
+      <c r="G20" s="181"/>
+      <c r="H20" s="181"/>
+      <c r="I20" s="181"/>
+      <c r="J20" s="181"/>
+      <c r="K20" s="182"/>
+      <c r="L20" s="180"/>
+      <c r="M20" s="181"/>
+      <c r="N20" s="182"/>
     </row>
     <row r="21" spans="1:14" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C21" s="145" t="s">
@@ -4068,7 +4068,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
@@ -4078,58 +4078,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C1" s="199" t="s">
+      <c r="C1" s="201" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="199"/>
-      <c r="E1" s="199"/>
-      <c r="F1" s="199"/>
+      <c r="D1" s="201"/>
+      <c r="E1" s="201"/>
+      <c r="F1" s="201"/>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="199"/>
-      <c r="D2" s="199"/>
-      <c r="E2" s="199"/>
-      <c r="F2" s="199"/>
+      <c r="C2" s="201"/>
+      <c r="D2" s="201"/>
+      <c r="E2" s="201"/>
+      <c r="F2" s="201"/>
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="199"/>
-      <c r="D3" s="199"/>
-      <c r="E3" s="199"/>
-      <c r="F3" s="199"/>
+      <c r="C3" s="201"/>
+      <c r="D3" s="201"/>
+      <c r="E3" s="201"/>
+      <c r="F3" s="201"/>
     </row>
     <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="200"/>
-      <c r="D4" s="200"/>
-      <c r="E4" s="200"/>
-      <c r="F4" s="200"/>
+      <c r="C4" s="202"/>
+      <c r="D4" s="202"/>
+      <c r="E4" s="202"/>
+      <c r="F4" s="202"/>
     </row>
     <row r="5" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A5" s="201" t="s">
+      <c r="A5" s="200" t="s">
         <v>99</v>
       </c>
-      <c r="B5" s="201"/>
-      <c r="C5" s="201"/>
-      <c r="D5" s="201"/>
-      <c r="E5" s="201"/>
-      <c r="F5" s="201"/>
+      <c r="B5" s="200"/>
+      <c r="C5" s="200"/>
+      <c r="D5" s="200"/>
+      <c r="E5" s="200"/>
+      <c r="F5" s="200"/>
     </row>
     <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="202" t="s">
+      <c r="A6" s="146" t="s">
         <v>97</v>
       </c>
-      <c r="B6" s="202" t="s">
+      <c r="B6" s="146" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="202" t="s">
+      <c r="C6" s="146" t="s">
         <v>100</v>
       </c>
-      <c r="D6" s="202" t="s">
+      <c r="D6" s="146" t="s">
         <v>93</v>
       </c>
-      <c r="E6" s="202" t="s">
+      <c r="E6" s="146" t="s">
         <v>59</v>
       </c>
-      <c r="F6" s="202" t="s">
+      <c r="F6" s="146" t="s">
         <v>98</v>
       </c>
     </row>

</xml_diff>

<commit_message>
AgregarRecetaTerminado y un Poco menusemanal
</commit_message>
<xml_diff>
--- a/ExcelAddIn1/Resources/FICHA RECETA.xlsx
+++ b/ExcelAddIn1/Resources/FICHA RECETA.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MANOLO\Documents\GitHub\VSTOexcelRest\ExcelAddIn1\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Documents\GitHub\VSTOexcelRest\ExcelAddIn1\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19560" windowHeight="8340" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19560" windowHeight="8340" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="ReporteInventario" sheetId="3" r:id="rId1"/>
@@ -17,7 +17,8 @@
     <sheet name="Receta" sheetId="1" r:id="rId3"/>
     <sheet name="ReporterCocina" sheetId="5" r:id="rId4"/>
     <sheet name="DetalleReceta" sheetId="6" r:id="rId5"/>
-    <sheet name="Congelados" sheetId="7" r:id="rId6"/>
+    <sheet name="IngredientesMenuDia" sheetId="8" r:id="rId6"/>
+    <sheet name="Congelados" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="CANTIDAD_A_ELABORAR">Receta!$J$4</definedName>
@@ -29,6 +30,7 @@
     <definedName name="FECHA_FIN_IMP">ReporteInventarioImprimir!$I$2</definedName>
     <definedName name="FECHA_INI_IMP">ReporteInventarioImprimir!$I$1</definedName>
     <definedName name="LITROS_A_ELABORAR">Receta!$J$3</definedName>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="MARGEN_ANTERIOR">Receta!$J$11</definedName>
     <definedName name="MARGEN_PRODUCTO">Receta!$J$12</definedName>
     <definedName name="NOMBRE">Receta!$B$2</definedName>
@@ -48,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="105">
   <si>
     <t>Receta</t>
   </si>
@@ -373,6 +375,18 @@
   <si>
     <t>Descipción</t>
   </si>
+  <si>
+    <t>Almacenes Mercatto                                                   S. de R.L. de C.V.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fecha </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ingredientes del Menú Semanal </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clave        Ingrediente </t>
+  </si>
 </sst>
 </file>
 
@@ -385,7 +399,7 @@
     <numFmt numFmtId="165" formatCode="0.000%"/>
     <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -564,6 +578,21 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial Black"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="14">
     <fill>
@@ -1117,7 +1146,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="203">
+  <cellXfs count="217">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1607,6 +1636,27 @@
     <xf numFmtId="0" fontId="23" fillId="13" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -1791,6 +1841,10 @@
     <xf numFmtId="0" fontId="17" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="13" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1800,6 +1854,18 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -1820,7 +1886,9 @@
       </font>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="0"/>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1882,6 +1950,55 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1476375</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>16972</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="1476375" cy="712297"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -2396,45 +2513,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="148" t="s">
+      <c r="B1" s="155" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="148"/>
-      <c r="D1" s="148"/>
-      <c r="E1" s="148"/>
-      <c r="F1" s="148"/>
+      <c r="C1" s="155"/>
+      <c r="D1" s="155"/>
+      <c r="E1" s="155"/>
+      <c r="F1" s="155"/>
       <c r="G1" s="66" t="s">
         <v>54</v>
       </c>
       <c r="H1" s="66"/>
-      <c r="I1" s="149">
+      <c r="I1" s="156">
         <v>42491</v>
       </c>
-      <c r="J1" s="149"/>
+      <c r="J1" s="156"/>
     </row>
     <row r="2" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="148"/>
-      <c r="C2" s="148"/>
-      <c r="D2" s="148"/>
-      <c r="E2" s="148"/>
-      <c r="F2" s="148"/>
+      <c r="B2" s="155"/>
+      <c r="C2" s="155"/>
+      <c r="D2" s="155"/>
+      <c r="E2" s="155"/>
+      <c r="F2" s="155"/>
       <c r="G2" s="68" t="s">
         <v>55</v>
       </c>
       <c r="H2" s="68"/>
-      <c r="I2" s="149">
+      <c r="I2" s="156">
         <v>42639</v>
       </c>
-      <c r="J2" s="149"/>
+      <c r="J2" s="156"/>
     </row>
     <row r="3" spans="1:10" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="147" t="s">
+      <c r="B3" s="154" t="s">
         <v>56</v>
       </c>
-      <c r="C3" s="147"/>
-      <c r="D3" s="147"/>
-      <c r="E3" s="147"/>
-      <c r="F3" s="147"/>
+      <c r="C3" s="154"/>
+      <c r="D3" s="154"/>
+      <c r="E3" s="154"/>
+      <c r="F3" s="154"/>
       <c r="G3" s="67"/>
       <c r="H3" s="67"/>
       <c r="I3" s="65"/>
@@ -2574,7 +2691,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -2592,52 +2709,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="169" t="s">
+      <c r="A1" s="176" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="160" t="s">
+      <c r="B1" s="167" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="161"/>
-      <c r="D1" s="161"/>
-      <c r="E1" s="161"/>
-      <c r="F1" s="162"/>
+      <c r="C1" s="168"/>
+      <c r="D1" s="168"/>
+      <c r="E1" s="168"/>
+      <c r="F1" s="169"/>
       <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="170"/>
-      <c r="B2" s="163" t="s">
+      <c r="A2" s="177"/>
+      <c r="B2" s="170" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="164"/>
-      <c r="D2" s="164"/>
-      <c r="E2" s="164"/>
-      <c r="F2" s="165"/>
-      <c r="G2" s="152" t="s">
+      <c r="C2" s="171"/>
+      <c r="D2" s="171"/>
+      <c r="E2" s="171"/>
+      <c r="F2" s="172"/>
+      <c r="G2" s="159" t="s">
         <v>47</v>
       </c>
-      <c r="H2" s="156" t="s">
+      <c r="H2" s="163" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="157"/>
+      <c r="I2" s="164"/>
       <c r="J2" s="19">
         <v>0.85</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="171"/>
-      <c r="B3" s="166"/>
-      <c r="C3" s="167"/>
-      <c r="D3" s="167"/>
-      <c r="E3" s="167"/>
-      <c r="F3" s="168"/>
-      <c r="G3" s="153"/>
-      <c r="H3" s="156" t="s">
+      <c r="A3" s="178"/>
+      <c r="B3" s="173"/>
+      <c r="C3" s="174"/>
+      <c r="D3" s="174"/>
+      <c r="E3" s="174"/>
+      <c r="F3" s="175"/>
+      <c r="G3" s="160"/>
+      <c r="H3" s="163" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="157"/>
+      <c r="I3" s="164"/>
       <c r="J3" s="20">
         <v>10</v>
       </c>
@@ -2664,10 +2781,10 @@
       <c r="G4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="158" t="s">
+      <c r="H4" s="165" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="159"/>
+      <c r="I4" s="166"/>
       <c r="J4" s="23">
         <v>8.5</v>
       </c>
@@ -2680,10 +2797,10 @@
       <c r="E5" s="24"/>
       <c r="F5" s="26"/>
       <c r="G5" s="26"/>
-      <c r="H5" s="154" t="s">
+      <c r="H5" s="161" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="155"/>
+      <c r="I5" s="162"/>
       <c r="J5" s="27">
         <f>SUM(G5:G100)</f>
         <v>0</v>
@@ -2697,10 +2814,10 @@
       <c r="E6" s="24"/>
       <c r="F6" s="26"/>
       <c r="G6" s="26"/>
-      <c r="H6" s="154" t="s">
+      <c r="H6" s="161" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="155"/>
+      <c r="I6" s="162"/>
       <c r="J6" s="28">
         <f>J5*0.05</f>
         <v>0</v>
@@ -2714,10 +2831,10 @@
       <c r="E7" s="24"/>
       <c r="F7" s="26"/>
       <c r="G7" s="26"/>
-      <c r="H7" s="154" t="s">
+      <c r="H7" s="161" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="155"/>
+      <c r="I7" s="162"/>
       <c r="J7" s="28">
         <v>110</v>
       </c>
@@ -2730,10 +2847,10 @@
       <c r="E8" s="24"/>
       <c r="F8" s="26"/>
       <c r="G8" s="26"/>
-      <c r="H8" s="154" t="s">
+      <c r="H8" s="161" t="s">
         <v>14</v>
       </c>
-      <c r="I8" s="155"/>
+      <c r="I8" s="162"/>
       <c r="J8" s="29">
         <v>150</v>
       </c>
@@ -2746,10 +2863,10 @@
       <c r="E9" s="24"/>
       <c r="F9" s="26"/>
       <c r="G9" s="26"/>
-      <c r="H9" s="154" t="s">
+      <c r="H9" s="161" t="s">
         <v>15</v>
       </c>
-      <c r="I9" s="154"/>
+      <c r="I9" s="161"/>
       <c r="J9" s="30">
         <f>(PRECIO_VENTA*LITROS_A_ELABORAR)</f>
         <v>1500</v>
@@ -2763,10 +2880,10 @@
       <c r="E10" s="24"/>
       <c r="F10" s="26"/>
       <c r="G10" s="26"/>
-      <c r="H10" s="154" t="s">
+      <c r="H10" s="161" t="s">
         <v>16</v>
       </c>
-      <c r="I10" s="154"/>
+      <c r="I10" s="161"/>
       <c r="J10" s="31">
         <f>J9-COSTO_TOTAL_MATERIA_PRIMA</f>
         <v>1500</v>
@@ -2780,10 +2897,10 @@
       <c r="E11" s="24"/>
       <c r="F11" s="26"/>
       <c r="G11" s="26"/>
-      <c r="H11" s="150" t="s">
+      <c r="H11" s="157" t="s">
         <v>19</v>
       </c>
-      <c r="I11" s="151"/>
+      <c r="I11" s="158"/>
       <c r="J11" s="32">
         <v>0.27</v>
       </c>
@@ -2796,10 +2913,10 @@
       <c r="E12" s="24"/>
       <c r="F12" s="26"/>
       <c r="G12" s="26"/>
-      <c r="H12" s="150" t="s">
+      <c r="H12" s="157" t="s">
         <v>20</v>
       </c>
-      <c r="I12" s="151"/>
+      <c r="I12" s="158"/>
       <c r="J12" s="32">
         <f>((J5+COSTO_PREPARACION)/J9-1)*(-1)</f>
         <v>0.92666666666666664</v>
@@ -2904,8 +3021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2939,22 +3056,22 @@
       <c r="N1" s="81"/>
       <c r="O1" s="81"/>
       <c r="P1" s="81"/>
-      <c r="Q1" s="172" t="s">
+      <c r="Q1" s="179" t="s">
         <v>60</v>
       </c>
-      <c r="R1" s="173"/>
-      <c r="S1" s="172" t="s">
+      <c r="R1" s="180"/>
+      <c r="S1" s="179" t="s">
         <v>61</v>
       </c>
-      <c r="T1" s="173"/>
-      <c r="U1" s="172" t="s">
+      <c r="T1" s="180"/>
+      <c r="U1" s="179" t="s">
         <v>62</v>
       </c>
-      <c r="V1" s="173"/>
-      <c r="W1" s="172" t="s">
+      <c r="V1" s="180"/>
+      <c r="W1" s="179" t="s">
         <v>63</v>
       </c>
-      <c r="X1" s="173"/>
+      <c r="X1" s="180"/>
       <c r="Y1" s="81"/>
       <c r="Z1" s="81"/>
       <c r="AA1" s="81"/>
@@ -3654,7 +3771,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M7" sqref="M7:N7"/>
     </sheetView>
   </sheetViews>
@@ -3670,36 +3787,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="199"/>
-      <c r="B1" s="199"/>
-      <c r="C1" s="199"/>
-      <c r="D1" s="199"/>
-      <c r="E1" s="199"/>
-      <c r="F1" s="199"/>
-      <c r="G1" s="199"/>
-      <c r="H1" s="199"/>
-      <c r="I1" s="199"/>
-      <c r="J1" s="199"/>
-      <c r="K1" s="199"/>
-      <c r="L1" s="199"/>
-      <c r="M1" s="199"/>
-      <c r="N1" s="199"/>
+      <c r="A1" s="206"/>
+      <c r="B1" s="206"/>
+      <c r="C1" s="206"/>
+      <c r="D1" s="206"/>
+      <c r="E1" s="206"/>
+      <c r="F1" s="206"/>
+      <c r="G1" s="206"/>
+      <c r="H1" s="206"/>
+      <c r="I1" s="206"/>
+      <c r="J1" s="206"/>
+      <c r="K1" s="206"/>
+      <c r="L1" s="206"/>
+      <c r="M1" s="206"/>
+      <c r="N1" s="206"/>
     </row>
     <row r="2" spans="1:16" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="199"/>
-      <c r="B2" s="199"/>
-      <c r="C2" s="199"/>
-      <c r="D2" s="199"/>
-      <c r="E2" s="199"/>
-      <c r="F2" s="199"/>
-      <c r="G2" s="199"/>
-      <c r="H2" s="199"/>
-      <c r="I2" s="199"/>
-      <c r="J2" s="199"/>
-      <c r="K2" s="199"/>
-      <c r="L2" s="199"/>
-      <c r="M2" s="199"/>
-      <c r="N2" s="199"/>
+      <c r="A2" s="206"/>
+      <c r="B2" s="206"/>
+      <c r="C2" s="206"/>
+      <c r="D2" s="206"/>
+      <c r="E2" s="206"/>
+      <c r="F2" s="206"/>
+      <c r="G2" s="206"/>
+      <c r="H2" s="206"/>
+      <c r="I2" s="206"/>
+      <c r="J2" s="206"/>
+      <c r="K2" s="206"/>
+      <c r="L2" s="206"/>
+      <c r="M2" s="206"/>
+      <c r="N2" s="206"/>
     </row>
     <row r="3" spans="1:16" s="133" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="134"/>
@@ -3721,8 +3838,8 @@
       <c r="A4" s="135" t="s">
         <v>80</v>
       </c>
-      <c r="B4" s="193"/>
-      <c r="C4" s="193"/>
+      <c r="B4" s="200"/>
+      <c r="C4" s="200"/>
       <c r="D4" s="96"/>
       <c r="E4" s="96"/>
       <c r="F4" s="140" t="s">
@@ -3731,11 +3848,11 @@
       <c r="G4" s="140" t="s">
         <v>81</v>
       </c>
-      <c r="H4" s="186" t="s">
+      <c r="H4" s="193" t="s">
         <v>82</v>
       </c>
-      <c r="I4" s="186"/>
-      <c r="J4" s="186"/>
+      <c r="I4" s="193"/>
+      <c r="J4" s="193"/>
       <c r="K4" s="141" t="s">
         <v>83</v>
       </c>
@@ -3751,7 +3868,7 @@
       <c r="P4" s="110"/>
     </row>
     <row r="5" spans="1:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="194" t="s">
+      <c r="A5" s="201" t="s">
         <v>86</v>
       </c>
       <c r="B5" s="97"/>
@@ -3762,8 +3879,8 @@
       <c r="E5" s="98"/>
       <c r="F5" s="99"/>
       <c r="G5" s="100"/>
-      <c r="H5" s="187"/>
-      <c r="I5" s="188"/>
+      <c r="H5" s="194"/>
+      <c r="I5" s="195"/>
       <c r="J5" s="101"/>
       <c r="K5" s="100"/>
       <c r="L5" s="102"/>
@@ -3771,7 +3888,7 @@
       <c r="N5" s="104"/>
     </row>
     <row r="6" spans="1:16" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="195"/>
+      <c r="A6" s="202"/>
       <c r="B6" s="107"/>
       <c r="C6" s="109" t="s">
         <v>88</v>
@@ -3784,17 +3901,17 @@
       <c r="G6" s="140" t="s">
         <v>90</v>
       </c>
-      <c r="H6" s="189" t="s">
+      <c r="H6" s="196" t="s">
         <v>91</v>
       </c>
-      <c r="I6" s="190"/>
-      <c r="J6" s="190"/>
-      <c r="K6" s="190"/>
-      <c r="L6" s="191"/>
-      <c r="M6" s="196" t="s">
+      <c r="I6" s="197"/>
+      <c r="J6" s="197"/>
+      <c r="K6" s="197"/>
+      <c r="L6" s="198"/>
+      <c r="M6" s="203" t="s">
         <v>35</v>
       </c>
-      <c r="N6" s="197"/>
+      <c r="N6" s="204"/>
     </row>
     <row r="7" spans="1:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="136" t="s">
@@ -3812,13 +3929,13 @@
       <c r="E7" s="112"/>
       <c r="F7" s="121"/>
       <c r="G7" s="105"/>
-      <c r="H7" s="187"/>
-      <c r="I7" s="188"/>
-      <c r="J7" s="188"/>
-      <c r="K7" s="188"/>
-      <c r="L7" s="192"/>
-      <c r="M7" s="198"/>
-      <c r="N7" s="198"/>
+      <c r="H7" s="194"/>
+      <c r="I7" s="195"/>
+      <c r="J7" s="195"/>
+      <c r="K7" s="195"/>
+      <c r="L7" s="199"/>
+      <c r="M7" s="205"/>
+      <c r="N7" s="205"/>
     </row>
     <row r="8" spans="1:16" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="122"/>
@@ -3842,19 +3959,19 @@
       <c r="C9" s="126"/>
       <c r="D9" s="127"/>
       <c r="E9" s="113"/>
-      <c r="F9" s="183" t="s">
+      <c r="F9" s="190" t="s">
         <v>0</v>
       </c>
-      <c r="G9" s="184"/>
-      <c r="H9" s="184"/>
-      <c r="I9" s="184"/>
-      <c r="J9" s="184"/>
-      <c r="K9" s="185"/>
-      <c r="L9" s="183" t="s">
+      <c r="G9" s="191"/>
+      <c r="H9" s="191"/>
+      <c r="I9" s="191"/>
+      <c r="J9" s="191"/>
+      <c r="K9" s="192"/>
+      <c r="L9" s="190" t="s">
         <v>94</v>
       </c>
-      <c r="M9" s="184"/>
-      <c r="N9" s="185"/>
+      <c r="M9" s="191"/>
+      <c r="N9" s="192"/>
     </row>
     <row r="10" spans="1:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="124"/>
@@ -3862,15 +3979,15 @@
       <c r="C10" s="128"/>
       <c r="D10" s="129"/>
       <c r="E10" s="113"/>
-      <c r="F10" s="174"/>
-      <c r="G10" s="175"/>
-      <c r="H10" s="175"/>
-      <c r="I10" s="175"/>
-      <c r="J10" s="175"/>
-      <c r="K10" s="176"/>
-      <c r="L10" s="174"/>
-      <c r="M10" s="175"/>
-      <c r="N10" s="176"/>
+      <c r="F10" s="181"/>
+      <c r="G10" s="182"/>
+      <c r="H10" s="182"/>
+      <c r="I10" s="182"/>
+      <c r="J10" s="182"/>
+      <c r="K10" s="183"/>
+      <c r="L10" s="181"/>
+      <c r="M10" s="182"/>
+      <c r="N10" s="183"/>
     </row>
     <row r="11" spans="1:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="124"/>
@@ -3878,15 +3995,15 @@
       <c r="C11" s="128"/>
       <c r="D11" s="129"/>
       <c r="E11" s="113"/>
-      <c r="F11" s="177"/>
-      <c r="G11" s="178"/>
-      <c r="H11" s="178"/>
-      <c r="I11" s="178"/>
-      <c r="J11" s="178"/>
-      <c r="K11" s="179"/>
-      <c r="L11" s="177"/>
-      <c r="M11" s="178"/>
-      <c r="N11" s="179"/>
+      <c r="F11" s="184"/>
+      <c r="G11" s="185"/>
+      <c r="H11" s="185"/>
+      <c r="I11" s="185"/>
+      <c r="J11" s="185"/>
+      <c r="K11" s="186"/>
+      <c r="L11" s="184"/>
+      <c r="M11" s="185"/>
+      <c r="N11" s="186"/>
     </row>
     <row r="12" spans="1:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="124"/>
@@ -3894,15 +4011,15 @@
       <c r="C12" s="128"/>
       <c r="D12" s="129"/>
       <c r="E12" s="113"/>
-      <c r="F12" s="177"/>
-      <c r="G12" s="178"/>
-      <c r="H12" s="178"/>
-      <c r="I12" s="178"/>
-      <c r="J12" s="178"/>
-      <c r="K12" s="179"/>
-      <c r="L12" s="177"/>
-      <c r="M12" s="178"/>
-      <c r="N12" s="179"/>
+      <c r="F12" s="184"/>
+      <c r="G12" s="185"/>
+      <c r="H12" s="185"/>
+      <c r="I12" s="185"/>
+      <c r="J12" s="185"/>
+      <c r="K12" s="186"/>
+      <c r="L12" s="184"/>
+      <c r="M12" s="185"/>
+      <c r="N12" s="186"/>
     </row>
     <row r="13" spans="1:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="124"/>
@@ -3910,15 +4027,15 @@
       <c r="C13" s="126"/>
       <c r="D13" s="127"/>
       <c r="E13" s="113"/>
-      <c r="F13" s="177"/>
-      <c r="G13" s="178"/>
-      <c r="H13" s="178"/>
-      <c r="I13" s="178"/>
-      <c r="J13" s="178"/>
-      <c r="K13" s="179"/>
-      <c r="L13" s="177"/>
-      <c r="M13" s="178"/>
-      <c r="N13" s="179"/>
+      <c r="F13" s="184"/>
+      <c r="G13" s="185"/>
+      <c r="H13" s="185"/>
+      <c r="I13" s="185"/>
+      <c r="J13" s="185"/>
+      <c r="K13" s="186"/>
+      <c r="L13" s="184"/>
+      <c r="M13" s="185"/>
+      <c r="N13" s="186"/>
     </row>
     <row r="14" spans="1:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="124"/>
@@ -3926,15 +4043,15 @@
       <c r="C14" s="126"/>
       <c r="D14" s="127"/>
       <c r="E14" s="113"/>
-      <c r="F14" s="177"/>
-      <c r="G14" s="178"/>
-      <c r="H14" s="178"/>
-      <c r="I14" s="178"/>
-      <c r="J14" s="178"/>
-      <c r="K14" s="179"/>
-      <c r="L14" s="177"/>
-      <c r="M14" s="178"/>
-      <c r="N14" s="179"/>
+      <c r="F14" s="184"/>
+      <c r="G14" s="185"/>
+      <c r="H14" s="185"/>
+      <c r="I14" s="185"/>
+      <c r="J14" s="185"/>
+      <c r="K14" s="186"/>
+      <c r="L14" s="184"/>
+      <c r="M14" s="185"/>
+      <c r="N14" s="186"/>
     </row>
     <row r="15" spans="1:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="124"/>
@@ -3942,15 +4059,15 @@
       <c r="C15" s="126"/>
       <c r="D15" s="127"/>
       <c r="E15" s="113"/>
-      <c r="F15" s="177"/>
-      <c r="G15" s="178"/>
-      <c r="H15" s="178"/>
-      <c r="I15" s="178"/>
-      <c r="J15" s="178"/>
-      <c r="K15" s="179"/>
-      <c r="L15" s="177"/>
-      <c r="M15" s="178"/>
-      <c r="N15" s="179"/>
+      <c r="F15" s="184"/>
+      <c r="G15" s="185"/>
+      <c r="H15" s="185"/>
+      <c r="I15" s="185"/>
+      <c r="J15" s="185"/>
+      <c r="K15" s="186"/>
+      <c r="L15" s="184"/>
+      <c r="M15" s="185"/>
+      <c r="N15" s="186"/>
     </row>
     <row r="16" spans="1:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="124"/>
@@ -3958,15 +4075,15 @@
       <c r="C16" s="126"/>
       <c r="D16" s="127"/>
       <c r="E16" s="113"/>
-      <c r="F16" s="177"/>
-      <c r="G16" s="178"/>
-      <c r="H16" s="178"/>
-      <c r="I16" s="178"/>
-      <c r="J16" s="178"/>
-      <c r="K16" s="179"/>
-      <c r="L16" s="177"/>
-      <c r="M16" s="178"/>
-      <c r="N16" s="179"/>
+      <c r="F16" s="184"/>
+      <c r="G16" s="185"/>
+      <c r="H16" s="185"/>
+      <c r="I16" s="185"/>
+      <c r="J16" s="185"/>
+      <c r="K16" s="186"/>
+      <c r="L16" s="184"/>
+      <c r="M16" s="185"/>
+      <c r="N16" s="186"/>
     </row>
     <row r="17" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="124"/>
@@ -3974,15 +4091,15 @@
       <c r="C17" s="126"/>
       <c r="D17" s="127"/>
       <c r="E17" s="113"/>
-      <c r="F17" s="177"/>
-      <c r="G17" s="178"/>
-      <c r="H17" s="178"/>
-      <c r="I17" s="178"/>
-      <c r="J17" s="178"/>
-      <c r="K17" s="179"/>
-      <c r="L17" s="177"/>
-      <c r="M17" s="178"/>
-      <c r="N17" s="179"/>
+      <c r="F17" s="184"/>
+      <c r="G17" s="185"/>
+      <c r="H17" s="185"/>
+      <c r="I17" s="185"/>
+      <c r="J17" s="185"/>
+      <c r="K17" s="186"/>
+      <c r="L17" s="184"/>
+      <c r="M17" s="185"/>
+      <c r="N17" s="186"/>
     </row>
     <row r="18" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="130"/>
@@ -3990,15 +4107,15 @@
       <c r="C18" s="126"/>
       <c r="D18" s="127"/>
       <c r="E18" s="113"/>
-      <c r="F18" s="177"/>
-      <c r="G18" s="178"/>
-      <c r="H18" s="178"/>
-      <c r="I18" s="178"/>
-      <c r="J18" s="178"/>
-      <c r="K18" s="179"/>
-      <c r="L18" s="177"/>
-      <c r="M18" s="178"/>
-      <c r="N18" s="179"/>
+      <c r="F18" s="184"/>
+      <c r="G18" s="185"/>
+      <c r="H18" s="185"/>
+      <c r="I18" s="185"/>
+      <c r="J18" s="185"/>
+      <c r="K18" s="186"/>
+      <c r="L18" s="184"/>
+      <c r="M18" s="185"/>
+      <c r="N18" s="186"/>
     </row>
     <row r="19" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="124" t="s">
@@ -4010,15 +4127,15 @@
       <c r="C19" s="126"/>
       <c r="D19" s="127"/>
       <c r="E19" s="113"/>
-      <c r="F19" s="177"/>
-      <c r="G19" s="178"/>
-      <c r="H19" s="178"/>
-      <c r="I19" s="178"/>
-      <c r="J19" s="178"/>
-      <c r="K19" s="179"/>
-      <c r="L19" s="177"/>
-      <c r="M19" s="178"/>
-      <c r="N19" s="179"/>
+      <c r="F19" s="184"/>
+      <c r="G19" s="185"/>
+      <c r="H19" s="185"/>
+      <c r="I19" s="185"/>
+      <c r="J19" s="185"/>
+      <c r="K19" s="186"/>
+      <c r="L19" s="184"/>
+      <c r="M19" s="185"/>
+      <c r="N19" s="186"/>
     </row>
     <row r="20" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="131"/>
@@ -4026,15 +4143,15 @@
       <c r="C20" s="126"/>
       <c r="D20" s="127"/>
       <c r="E20" s="113"/>
-      <c r="F20" s="180"/>
-      <c r="G20" s="181"/>
-      <c r="H20" s="181"/>
-      <c r="I20" s="181"/>
-      <c r="J20" s="181"/>
-      <c r="K20" s="182"/>
-      <c r="L20" s="180"/>
-      <c r="M20" s="181"/>
-      <c r="N20" s="182"/>
+      <c r="F20" s="187"/>
+      <c r="G20" s="188"/>
+      <c r="H20" s="188"/>
+      <c r="I20" s="188"/>
+      <c r="J20" s="188"/>
+      <c r="K20" s="189"/>
+      <c r="L20" s="187"/>
+      <c r="M20" s="188"/>
+      <c r="N20" s="189"/>
     </row>
     <row r="21" spans="1:14" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C21" s="145" t="s">
@@ -4066,10 +4183,290 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24" customWidth="1"/>
+    <col min="2" max="2" width="44.140625" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="207" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" s="207"/>
+      <c r="D1" s="147"/>
+      <c r="E1" s="147"/>
+    </row>
+    <row r="2" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="207"/>
+      <c r="C2" s="207"/>
+      <c r="D2" s="212"/>
+      <c r="E2" s="211"/>
+    </row>
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="207"/>
+      <c r="C3" s="207"/>
+      <c r="E3" s="148"/>
+    </row>
+    <row r="4" spans="1:5" ht="27.75" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B4" s="214" t="s">
+        <v>103</v>
+      </c>
+      <c r="C4" s="214"/>
+      <c r="D4" s="213"/>
+    </row>
+    <row r="5" spans="1:5" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="150" t="s">
+        <v>104</v>
+      </c>
+      <c r="B5" s="152" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="151" t="s">
+        <v>93</v>
+      </c>
+      <c r="D5" s="153" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="153" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="131"/>
+      <c r="B6" s="131"/>
+      <c r="C6" s="149"/>
+      <c r="D6" s="131"/>
+      <c r="E6" s="131"/>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="131"/>
+      <c r="B7" s="131"/>
+      <c r="C7" s="149"/>
+      <c r="D7" s="131"/>
+      <c r="E7" s="131"/>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="131"/>
+      <c r="B8" s="131"/>
+      <c r="C8" s="149"/>
+      <c r="D8" s="131"/>
+      <c r="E8" s="131"/>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="131"/>
+      <c r="B9" s="131"/>
+      <c r="C9" s="149"/>
+      <c r="D9" s="131"/>
+      <c r="E9" s="131"/>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="131"/>
+      <c r="B10" s="131"/>
+      <c r="C10" s="149"/>
+      <c r="D10" s="131"/>
+      <c r="E10" s="131"/>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="131"/>
+      <c r="B11" s="131"/>
+      <c r="C11" s="149"/>
+      <c r="D11" s="131"/>
+      <c r="E11" s="131"/>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="131"/>
+      <c r="B12" s="131"/>
+      <c r="C12" s="149"/>
+      <c r="D12" s="131"/>
+      <c r="E12" s="131"/>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="131"/>
+      <c r="B13" s="131"/>
+      <c r="C13" s="149"/>
+      <c r="D13" s="131"/>
+      <c r="E13" s="131"/>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="131"/>
+      <c r="B14" s="131"/>
+      <c r="C14" s="149"/>
+      <c r="D14" s="131"/>
+      <c r="E14" s="131"/>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="131"/>
+      <c r="B15" s="131"/>
+      <c r="C15" s="149"/>
+      <c r="D15" s="131"/>
+      <c r="E15" s="131"/>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="131"/>
+      <c r="B16" s="131"/>
+      <c r="C16" s="149"/>
+      <c r="D16" s="131"/>
+      <c r="E16" s="131"/>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="131"/>
+      <c r="B17" s="131"/>
+      <c r="C17" s="149"/>
+      <c r="D17" s="131"/>
+      <c r="E17" s="131"/>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="131"/>
+      <c r="B18" s="131"/>
+      <c r="C18" s="149"/>
+      <c r="D18" s="131"/>
+      <c r="E18" s="131"/>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="131"/>
+      <c r="B19" s="131"/>
+      <c r="C19" s="149"/>
+      <c r="D19" s="131"/>
+      <c r="E19" s="131"/>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="131"/>
+      <c r="B20" s="131"/>
+      <c r="C20" s="149"/>
+      <c r="D20" s="131"/>
+      <c r="E20" s="131"/>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="131"/>
+      <c r="B21" s="131"/>
+      <c r="C21" s="149"/>
+      <c r="D21" s="131"/>
+      <c r="E21" s="131"/>
+    </row>
+    <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="215"/>
+      <c r="B22" s="215"/>
+      <c r="C22" s="216"/>
+      <c r="D22" s="215"/>
+      <c r="E22" s="215"/>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="131"/>
+      <c r="B23" s="131"/>
+      <c r="C23" s="131"/>
+      <c r="D23" s="131"/>
+      <c r="E23" s="131"/>
+    </row>
+    <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="131"/>
+      <c r="B24" s="131"/>
+      <c r="C24" s="131"/>
+      <c r="D24" s="131"/>
+      <c r="E24" s="131"/>
+    </row>
+    <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="131"/>
+      <c r="B25" s="131"/>
+      <c r="C25" s="131"/>
+      <c r="D25" s="131"/>
+      <c r="E25" s="131"/>
+    </row>
+    <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="131"/>
+      <c r="B26" s="131"/>
+      <c r="C26" s="131"/>
+      <c r="D26" s="131"/>
+      <c r="E26" s="131"/>
+    </row>
+    <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="131"/>
+      <c r="B27" s="131"/>
+      <c r="C27" s="131"/>
+      <c r="D27" s="131"/>
+      <c r="E27" s="131"/>
+    </row>
+    <row r="28" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="131"/>
+      <c r="B28" s="131"/>
+      <c r="C28" s="131"/>
+      <c r="D28" s="131"/>
+      <c r="E28" s="131"/>
+    </row>
+    <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="131"/>
+      <c r="B29" s="131"/>
+      <c r="C29" s="131"/>
+      <c r="D29" s="131"/>
+      <c r="E29" s="131"/>
+    </row>
+    <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="131"/>
+      <c r="B30" s="131"/>
+      <c r="C30" s="131"/>
+      <c r="D30" s="131"/>
+      <c r="E30" s="131"/>
+    </row>
+    <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="131"/>
+      <c r="B31" s="131"/>
+      <c r="C31" s="131"/>
+      <c r="D31" s="131"/>
+      <c r="E31" s="131"/>
+    </row>
+    <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="131"/>
+      <c r="B32" s="131"/>
+      <c r="C32" s="131"/>
+      <c r="D32" s="131"/>
+      <c r="E32" s="131"/>
+    </row>
+    <row r="33" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="131"/>
+      <c r="B33" s="131"/>
+      <c r="C33" s="131"/>
+      <c r="D33" s="131"/>
+      <c r="E33" s="131"/>
+    </row>
+    <row r="34" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="131"/>
+      <c r="B34" s="131"/>
+      <c r="C34" s="131"/>
+      <c r="D34" s="131"/>
+      <c r="E34" s="131"/>
+    </row>
+    <row r="35" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="131"/>
+      <c r="B35" s="131"/>
+      <c r="C35" s="131"/>
+      <c r="D35" s="131"/>
+      <c r="E35" s="131"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:C3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="A5" sqref="A5:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4078,40 +4475,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C1" s="201" t="s">
+      <c r="C1" s="209" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="201"/>
-      <c r="E1" s="201"/>
-      <c r="F1" s="201"/>
+      <c r="D1" s="209"/>
+      <c r="E1" s="209"/>
+      <c r="F1" s="209"/>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="201"/>
-      <c r="D2" s="201"/>
-      <c r="E2" s="201"/>
-      <c r="F2" s="201"/>
+      <c r="C2" s="209"/>
+      <c r="D2" s="209"/>
+      <c r="E2" s="209"/>
+      <c r="F2" s="209"/>
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="201"/>
-      <c r="D3" s="201"/>
-      <c r="E3" s="201"/>
-      <c r="F3" s="201"/>
+      <c r="C3" s="209"/>
+      <c r="D3" s="209"/>
+      <c r="E3" s="209"/>
+      <c r="F3" s="209"/>
     </row>
     <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="202"/>
-      <c r="D4" s="202"/>
-      <c r="E4" s="202"/>
-      <c r="F4" s="202"/>
+      <c r="C4" s="210"/>
+      <c r="D4" s="210"/>
+      <c r="E4" s="210"/>
+      <c r="F4" s="210"/>
     </row>
     <row r="5" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A5" s="200" t="s">
+      <c r="A5" s="208" t="s">
         <v>99</v>
       </c>
-      <c r="B5" s="200"/>
-      <c r="C5" s="200"/>
-      <c r="D5" s="200"/>
-      <c r="E5" s="200"/>
-      <c r="F5" s="200"/>
+      <c r="B5" s="208"/>
+      <c r="C5" s="208"/>
+      <c r="D5" s="208"/>
+      <c r="E5" s="208"/>
+      <c r="F5" s="208"/>
     </row>
     <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="146" t="s">

</xml_diff>